<commit_message>
Phân loại các đối tượng (CSDL)
</commit_message>
<xml_diff>
--- a/Doccuments/Object/ObjectInfo.xlsx
+++ b/Doccuments/Object/ObjectInfo.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\android\Projects\iocome\Doccuments\Object\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="84" windowWidth="12420" windowHeight="5856"/>
+    <workbookView xWindow="480" yWindow="90" windowWidth="12420" windowHeight="5850" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="CSDL" sheetId="2" r:id="rId2"/>
+    <sheet name="SSS" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="207">
   <si>
     <t>Chi tiêu</t>
   </si>
@@ -205,13 +210,445 @@
   </si>
   <si>
     <t>HashMap&lt;1-12, List&lt;Item&gt;&gt;</t>
+  </si>
+  <si>
+    <t>Gia đình</t>
+  </si>
+  <si>
+    <t>Nhóm</t>
+  </si>
+  <si>
+    <t>Encode</t>
+  </si>
+  <si>
+    <t>Obj</t>
+  </si>
+  <si>
+    <t>Avatar</t>
+  </si>
+  <si>
+    <t>User admin</t>
+  </si>
+  <si>
+    <t>Thành viên</t>
+  </si>
+  <si>
+    <t>Cá nhân (admin)</t>
+  </si>
+  <si>
+    <t>Kinh doanh</t>
+  </si>
+  <si>
+    <t>Quản lý chi tiêu</t>
+  </si>
+  <si>
+    <t>Thời trang</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Thể thao</t>
+  </si>
+  <si>
+    <t>Trang trí</t>
+  </si>
+  <si>
+    <t>Khác...</t>
+  </si>
+  <si>
+    <t>Dịch vụ</t>
+  </si>
+  <si>
+    <t>Tiêu vặt</t>
+  </si>
+  <si>
+    <t>Sức khỏe</t>
+  </si>
+  <si>
+    <t>Items</t>
+  </si>
+  <si>
+    <t>Gạo</t>
+  </si>
+  <si>
+    <t>Bánh mỳ</t>
+  </si>
+  <si>
+    <t>Thịt</t>
+  </si>
+  <si>
+    <t>Cá</t>
+  </si>
+  <si>
+    <t>Thịt lợn</t>
+  </si>
+  <si>
+    <t>Thịt bò</t>
+  </si>
+  <si>
+    <t>Tôm</t>
+  </si>
+  <si>
+    <t>Gia vị</t>
+  </si>
+  <si>
+    <t>Snack</t>
+  </si>
+  <si>
+    <t>Bánh kẹo</t>
+  </si>
+  <si>
+    <t>Thịt gà</t>
+  </si>
+  <si>
+    <t>Sữa</t>
+  </si>
+  <si>
+    <t>Bột</t>
+  </si>
+  <si>
+    <t>Giầy dép</t>
+  </si>
+  <si>
+    <t>Túi xách</t>
+  </si>
+  <si>
+    <t>Mũ</t>
+  </si>
+  <si>
+    <t>Đồng hồ</t>
+  </si>
+  <si>
+    <t>Trang sức</t>
+  </si>
+  <si>
+    <t>Kính</t>
+  </si>
+  <si>
+    <t>Tóc</t>
+  </si>
+  <si>
+    <t>Móng tay</t>
+  </si>
+  <si>
+    <t>Móng chân</t>
+  </si>
+  <si>
+    <t>Mỹ phẩm</t>
+  </si>
+  <si>
+    <t>Massage</t>
+  </si>
+  <si>
+    <t>Gia dụng</t>
+  </si>
+  <si>
+    <t>Nhà bếp</t>
+  </si>
+  <si>
+    <t>Phòng ngủ</t>
+  </si>
+  <si>
+    <t>Đèn</t>
+  </si>
+  <si>
+    <t>Tivi</t>
+  </si>
+  <si>
+    <t>Tủ lạnh</t>
+  </si>
+  <si>
+    <t>Điều hòa</t>
+  </si>
+  <si>
+    <t>Bình nóng lạnh</t>
+  </si>
+  <si>
+    <t>Loa</t>
+  </si>
+  <si>
+    <t>Máy hút bụi</t>
+  </si>
+  <si>
+    <t>Phòng tắm</t>
+  </si>
+  <si>
+    <t>Phòng khách</t>
+  </si>
+  <si>
+    <t>Xe máy</t>
+  </si>
+  <si>
+    <t>Xe ô tô</t>
+  </si>
+  <si>
+    <t>Xe đạp</t>
+  </si>
+  <si>
+    <t>Xăng</t>
+  </si>
+  <si>
+    <t>Bảo dưỡng</t>
+  </si>
+  <si>
+    <t>Phương tiện</t>
+  </si>
+  <si>
+    <t>Taxi</t>
+  </si>
+  <si>
+    <t>Xe ôm</t>
+  </si>
+  <si>
+    <t>Xe bus</t>
+  </si>
+  <si>
+    <t>Máy bay</t>
+  </si>
+  <si>
+    <t>Tàu</t>
+  </si>
+  <si>
+    <t>Yoga</t>
+  </si>
+  <si>
+    <t>Da</t>
+  </si>
+  <si>
+    <t>Răng miệng</t>
+  </si>
+  <si>
+    <t>Thực phẩm CN</t>
+  </si>
+  <si>
+    <t>Công viên</t>
+  </si>
+  <si>
+    <t>Dã ngoại</t>
+  </si>
+  <si>
+    <t>Trò chơi</t>
+  </si>
+  <si>
+    <t>Xem phim</t>
+  </si>
+  <si>
+    <t>Tiệc tùng</t>
+  </si>
+  <si>
+    <t>Quán nhậu</t>
+  </si>
+  <si>
+    <t>Bar</t>
+  </si>
+  <si>
+    <t>Giaáo dục</t>
+  </si>
+  <si>
+    <t>Học phí</t>
+  </si>
+  <si>
+    <t>Dụng cụ học tập</t>
+  </si>
+  <si>
+    <t>Vở</t>
+  </si>
+  <si>
+    <t>Dụng cụ</t>
+  </si>
+  <si>
+    <t>Trang phục</t>
+  </si>
+  <si>
+    <t>Dụng cụ âm nhạc</t>
+  </si>
+  <si>
+    <t>Đàn</t>
+  </si>
+  <si>
+    <t>Sáo</t>
+  </si>
+  <si>
+    <t>Kèn</t>
+  </si>
+  <si>
+    <t>Máy thể dục</t>
+  </si>
+  <si>
+    <t>Tạ</t>
+  </si>
+  <si>
+    <t>Sà</t>
+  </si>
+  <si>
+    <t>Thuốc bổ</t>
+  </si>
+  <si>
+    <t>Thuốc</t>
+  </si>
+  <si>
+    <t>Dụng cụ y tế</t>
+  </si>
+  <si>
+    <t>Khám sức khỏe</t>
+  </si>
+  <si>
+    <t>Viện phí</t>
+  </si>
+  <si>
+    <t>Đồ dùng cá nhân</t>
+  </si>
+  <si>
+    <t>Vật nuôi</t>
+  </si>
+  <si>
+    <t>Tai nghe</t>
+  </si>
+  <si>
+    <t>Balo</t>
+  </si>
+  <si>
+    <t>Vali</t>
+  </si>
+  <si>
+    <t>Dầu gội</t>
+  </si>
+  <si>
+    <t>Sữa tắm</t>
+  </si>
+  <si>
+    <t>Khăn mặt</t>
+  </si>
+  <si>
+    <t>Kính mắt</t>
+  </si>
+  <si>
+    <t>Khẩu trang</t>
+  </si>
+  <si>
+    <t>Nước hoa</t>
+  </si>
+  <si>
+    <t>Thức ăn</t>
+  </si>
+  <si>
+    <t>Vật dụng</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>Ăn uống</t>
+  </si>
+  <si>
+    <t>Vé cửa</t>
+  </si>
+  <si>
+    <t>Đồ lưu niệm</t>
+  </si>
+  <si>
+    <t>Vé phương tiện</t>
+  </si>
+  <si>
+    <t>Vé tàu</t>
+  </si>
+  <si>
+    <t>Vé máy bay</t>
+  </si>
+  <si>
+    <t>Xăng xe</t>
+  </si>
+  <si>
+    <t>Cước điện thoại</t>
+  </si>
+  <si>
+    <t>Truyền hình cap</t>
+  </si>
+  <si>
+    <t>Vệ sinh</t>
+  </si>
+  <si>
+    <t>Bảo an</t>
+  </si>
+  <si>
+    <t>Giao hàng</t>
+  </si>
+  <si>
+    <t>Lắp đặt</t>
+  </si>
+  <si>
+    <t>Tu sửa</t>
+  </si>
+  <si>
+    <t>Nhà cửa</t>
+  </si>
+  <si>
+    <t>Mua sắm</t>
+  </si>
+  <si>
+    <t>Sinh hoạt</t>
+  </si>
+  <si>
+    <t>Điện</t>
+  </si>
+  <si>
+    <t>Nước</t>
+  </si>
+  <si>
+    <t>Đi lại</t>
+  </si>
+  <si>
+    <t>Sinh nhật</t>
+  </si>
+  <si>
+    <t>Chiêu đãi</t>
+  </si>
+  <si>
+    <t>Họ hàng</t>
+  </si>
+  <si>
+    <t>Bạn bè</t>
+  </si>
+  <si>
+    <t>Khác hàng</t>
+  </si>
+  <si>
+    <t>Đồ trang trí</t>
+  </si>
+  <si>
+    <t>Đèn trang trí</t>
+  </si>
+  <si>
+    <t>Loại BH</t>
+  </si>
+  <si>
+    <t>Khác..</t>
+  </si>
+  <si>
+    <t>Sản lượng</t>
+  </si>
+  <si>
+    <t>Giá</t>
+  </si>
+  <si>
+    <t>int (đ)</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>img</t>
+  </si>
+  <si>
+    <t>Sản phẩm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -232,8 +669,21 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -246,8 +696,56 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -270,16 +768,219 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -289,6 +990,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -337,7 +1041,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -372,7 +1076,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -583,24 +1287,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="8.85546875" style="1"/>
     <col min="6" max="6" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="15" width="8.88671875" style="1"/>
-    <col min="16" max="16" width="6.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.88671875" style="1"/>
+    <col min="7" max="7" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="15" width="8.85546875" style="1"/>
+    <col min="16" max="16" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -620,7 +1322,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -640,7 +1342,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -660,7 +1362,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -680,7 +1382,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -700,7 +1402,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -714,211 +1416,211 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="3"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="3"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="3"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="3"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="3"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="3"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="3"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="3"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="3"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B27" s="3"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="3"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B33" s="3"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B34" s="3"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B35" s="3"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B36" s="3"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B37" s="3"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B38" s="3"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B39" s="3"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B40" s="3"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B41" s="3"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>40</v>
       </c>
@@ -932,13 +1634,2287 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B4:AQ191"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:D10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="9.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="10.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B4" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4" s="20"/>
+      <c r="I4" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="M4" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="N4" s="13"/>
+      <c r="O4" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="T4" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="U4" s="38"/>
+      <c r="V4" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="W4" s="11"/>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="11"/>
+      <c r="AA4" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB4" s="15"/>
+      <c r="AC4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE4" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF4" s="41"/>
+      <c r="AG4" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH4" s="7"/>
+      <c r="AJ4" s="42" t="s">
+        <v>206</v>
+      </c>
+      <c r="AK4" s="42"/>
+      <c r="AL4" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="AM4" s="7"/>
+    </row>
+    <row r="5" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B5" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="M5" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="N5" s="14"/>
+      <c r="O5" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="T5" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="U5" s="14"/>
+      <c r="V5" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="7"/>
+      <c r="AA5" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB5" s="7"/>
+      <c r="AC5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE5" s="42" t="s">
+        <v>206</v>
+      </c>
+      <c r="AF5" s="42"/>
+      <c r="AG5" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH5" s="7"/>
+      <c r="AJ5" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="AK5" s="7"/>
+      <c r="AL5" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="AM5" s="7"/>
+    </row>
+    <row r="6" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B6" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="M6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="T6" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="U6" s="39"/>
+      <c r="V6" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="7"/>
+      <c r="AA6" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB6" s="7"/>
+      <c r="AC6" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="AE6" s="25"/>
+      <c r="AF6" s="25"/>
+      <c r="AG6" s="23"/>
+      <c r="AH6" s="23"/>
+      <c r="AJ6" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="AK6" s="7"/>
+      <c r="AL6" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="AM6" s="7"/>
+    </row>
+    <row r="7" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B7" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="M7" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="T7" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="U7" s="12"/>
+      <c r="V7" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="7"/>
+      <c r="AA7" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB7" s="7"/>
+      <c r="AC7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ7" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="AK7" s="7"/>
+      <c r="AL7" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="AM7" s="7"/>
+    </row>
+    <row r="8" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B8" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="M8" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="T8" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="U8" s="7"/>
+      <c r="V8" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="W8" s="7"/>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="7"/>
+    </row>
+    <row r="9" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="Q9" s="37"/>
+      <c r="R9" s="37"/>
+      <c r="S9" s="37"/>
+      <c r="T9" s="37"/>
+    </row>
+    <row r="10" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="Q10" s="24"/>
+      <c r="R10" s="24"/>
+      <c r="S10" s="24"/>
+      <c r="T10" s="24"/>
+    </row>
+    <row r="11" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="Q11" s="27"/>
+      <c r="R11" s="27"/>
+      <c r="S11" s="27"/>
+      <c r="T11" s="27"/>
+    </row>
+    <row r="12" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B12" s="35" t="s">
+        <v>171</v>
+      </c>
+      <c r="C12" s="40"/>
+      <c r="E12" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="F12" s="16"/>
+      <c r="G12" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="H12" s="12"/>
+      <c r="J12" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="K12" s="16"/>
+      <c r="L12" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="M12" s="12"/>
+      <c r="O12" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="R12" s="12"/>
+      <c r="S12" s="27"/>
+      <c r="T12" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="U12" s="16"/>
+      <c r="V12" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="W12" s="12"/>
+      <c r="Y12" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="Z12" s="16"/>
+      <c r="AA12" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB12" s="12"/>
+      <c r="AD12" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="AE12" s="16"/>
+      <c r="AF12" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="AG12" s="12"/>
+      <c r="AI12" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="AJ12" s="16"/>
+      <c r="AK12" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="AL12" s="12"/>
+      <c r="AN12" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="AO12" s="16"/>
+      <c r="AP12" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="AQ12" s="12"/>
+    </row>
+    <row r="13" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B13" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="10"/>
+      <c r="E13" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="30"/>
+      <c r="G13" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13" s="7"/>
+      <c r="J13" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="K13" s="22"/>
+      <c r="L13" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M13" s="7"/>
+      <c r="O13" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="P13" s="22"/>
+      <c r="Q13" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="R13" s="7"/>
+      <c r="S13" s="27"/>
+      <c r="T13" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="U13" s="22"/>
+      <c r="V13" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="W13" s="7"/>
+      <c r="Y13" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="Z13" s="22"/>
+      <c r="AA13" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="AB13" s="7"/>
+      <c r="AD13" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE13" s="22"/>
+      <c r="AF13" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG13" s="7"/>
+      <c r="AI13" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="AJ13" s="22"/>
+      <c r="AK13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL13" s="7"/>
+      <c r="AN13" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="AO13" s="22"/>
+      <c r="AP13" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="AQ13" s="7"/>
+    </row>
+    <row r="14" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B14" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H14" s="7"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="M14" s="7"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="R14" s="7"/>
+      <c r="S14" s="27"/>
+      <c r="T14" s="22"/>
+      <c r="U14" s="22"/>
+      <c r="V14" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="W14" s="7"/>
+      <c r="Y14" s="22"/>
+      <c r="Z14" s="22"/>
+      <c r="AA14" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="AB14" s="7"/>
+      <c r="AD14" s="22"/>
+      <c r="AE14" s="22"/>
+      <c r="AF14" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="AG14" s="7"/>
+      <c r="AI14" s="22"/>
+      <c r="AJ14" s="22"/>
+      <c r="AK14" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="AL14" s="7"/>
+      <c r="AN14" s="22"/>
+      <c r="AO14" s="22"/>
+      <c r="AP14" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="AQ14" s="7"/>
+    </row>
+    <row r="15" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B15" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" s="7"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M15" s="7"/>
+      <c r="O15" s="22"/>
+      <c r="P15" s="22"/>
+      <c r="Q15" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="R15" s="7"/>
+      <c r="S15" s="27"/>
+      <c r="T15" s="22"/>
+      <c r="U15" s="22"/>
+      <c r="V15" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="W15" s="7"/>
+      <c r="Y15" s="22"/>
+      <c r="Z15" s="22"/>
+      <c r="AA15" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB15" s="7"/>
+      <c r="AD15" s="22"/>
+      <c r="AE15" s="22"/>
+      <c r="AF15" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="AG15" s="7"/>
+      <c r="AI15" s="22"/>
+      <c r="AJ15" s="22"/>
+      <c r="AK15" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="AL15" s="7"/>
+      <c r="AN15" s="22"/>
+      <c r="AO15" s="22"/>
+      <c r="AP15" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="AQ15" s="7"/>
+    </row>
+    <row r="16" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B16" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" s="10"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H16" s="7"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="M16" s="7"/>
+      <c r="O16" s="22"/>
+      <c r="P16" s="22"/>
+      <c r="Q16" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="R16" s="7"/>
+      <c r="T16" s="22"/>
+      <c r="U16" s="22"/>
+      <c r="V16" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="W16" s="7"/>
+      <c r="Y16" s="22"/>
+      <c r="Z16" s="22"/>
+      <c r="AA16" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB16" s="7"/>
+      <c r="AD16" s="22"/>
+      <c r="AE16" s="22"/>
+      <c r="AF16" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="AG16" s="7"/>
+      <c r="AI16" s="22"/>
+      <c r="AJ16" s="22"/>
+      <c r="AK16" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="AL16" s="7"/>
+      <c r="AN16" s="22"/>
+      <c r="AO16" s="22"/>
+      <c r="AP16" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="AQ16" s="7"/>
+    </row>
+    <row r="17" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B17" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H17" s="7"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="M17" s="7"/>
+      <c r="O17" s="22"/>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="R17" s="10"/>
+      <c r="T17" s="22"/>
+      <c r="U17" s="22"/>
+      <c r="V17" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="W17" s="7"/>
+      <c r="Y17" s="22"/>
+      <c r="Z17" s="22"/>
+      <c r="AA17" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB17" s="7"/>
+      <c r="AD17" s="22"/>
+      <c r="AE17" s="22"/>
+      <c r="AF17" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="AG17" s="7"/>
+      <c r="AI17" s="22"/>
+      <c r="AJ17" s="22"/>
+      <c r="AK17" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="AL17" s="7"/>
+      <c r="AN17" s="22"/>
+      <c r="AO17" s="22"/>
+      <c r="AP17" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="AQ17" s="7"/>
+    </row>
+    <row r="18" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B18" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H18" s="7"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="M18" s="7"/>
+      <c r="O18" s="22"/>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="R18" s="7"/>
+      <c r="T18" s="22"/>
+      <c r="U18" s="22"/>
+      <c r="V18" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="W18" s="7"/>
+      <c r="Y18" s="22"/>
+      <c r="Z18" s="22"/>
+      <c r="AA18" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB18" s="7"/>
+      <c r="AD18" s="22"/>
+      <c r="AE18" s="22"/>
+      <c r="AF18" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AG18" s="7"/>
+      <c r="AI18" s="22"/>
+      <c r="AJ18" s="22"/>
+      <c r="AK18" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL18" s="7"/>
+      <c r="AN18" s="22"/>
+      <c r="AO18" s="22"/>
+      <c r="AP18" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="AQ18" s="7"/>
+    </row>
+    <row r="19" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B19" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="H19" s="7"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="M19" s="7"/>
+      <c r="O19" s="22"/>
+      <c r="P19" s="22"/>
+      <c r="Q19" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="R19" s="7"/>
+      <c r="T19" s="22"/>
+      <c r="U19" s="22"/>
+      <c r="V19" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="W19" s="7"/>
+      <c r="Y19" s="22"/>
+      <c r="Z19" s="22"/>
+      <c r="AA19" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="AB19" s="7"/>
+      <c r="AD19" s="22"/>
+      <c r="AE19" s="22"/>
+      <c r="AF19" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG19" s="7"/>
+      <c r="AI19" s="22"/>
+      <c r="AJ19" s="22"/>
+      <c r="AK19" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL19" s="7"/>
+      <c r="AN19" s="22"/>
+      <c r="AO19" s="22"/>
+      <c r="AP19" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="AQ19" s="7"/>
+    </row>
+    <row r="20" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B20" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" s="10"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="H20" s="7"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="M20" s="7"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="22"/>
+      <c r="Q20" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="R20" s="7"/>
+      <c r="T20" s="22"/>
+      <c r="U20" s="22"/>
+      <c r="V20" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="W20" s="7"/>
+      <c r="Y20" s="22"/>
+      <c r="Z20" s="22"/>
+      <c r="AA20" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="AB20" s="7"/>
+      <c r="AD20" s="22"/>
+      <c r="AE20" s="22"/>
+      <c r="AF20" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="AG20" s="7"/>
+      <c r="AI20" s="22"/>
+      <c r="AJ20" s="22"/>
+      <c r="AK20" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL20" s="7"/>
+      <c r="AN20" s="22"/>
+      <c r="AO20" s="22"/>
+      <c r="AP20" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="AQ20" s="7"/>
+    </row>
+    <row r="21" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B21" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="10"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H21" s="7"/>
+      <c r="O21" s="22"/>
+      <c r="P21" s="22"/>
+      <c r="Q21" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="R21" s="10"/>
+      <c r="T21" s="22"/>
+      <c r="U21" s="22"/>
+      <c r="V21" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="W21" s="7"/>
+      <c r="Y21" s="22"/>
+      <c r="Z21" s="22"/>
+      <c r="AA21" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB21" s="7"/>
+      <c r="AD21" s="22"/>
+      <c r="AE21" s="22"/>
+      <c r="AF21" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="AG21" s="7"/>
+      <c r="AI21" s="22"/>
+      <c r="AJ21" s="22"/>
+      <c r="AK21" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL21" s="7"/>
+    </row>
+    <row r="22" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B22" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" s="10"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H22" s="7"/>
+      <c r="J22" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="K22" s="16"/>
+      <c r="L22" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="M22" s="12"/>
+      <c r="O22" s="22"/>
+      <c r="P22" s="22"/>
+      <c r="Q22" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="R22" s="10"/>
+      <c r="S22" s="26"/>
+      <c r="T22" s="22"/>
+      <c r="U22" s="22"/>
+      <c r="V22" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="W22" s="7"/>
+      <c r="Y22" s="22"/>
+      <c r="Z22" s="22"/>
+      <c r="AA22" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB22" s="7"/>
+      <c r="AD22" s="22"/>
+      <c r="AE22" s="22"/>
+      <c r="AF22" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AG22" s="7"/>
+    </row>
+    <row r="23" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B23" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="10"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="H23" s="7"/>
+      <c r="J23" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="K23" s="22"/>
+      <c r="L23" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="M23" s="7"/>
+      <c r="O23" s="22"/>
+      <c r="P23" s="22"/>
+      <c r="Q23" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="R23" s="10"/>
+      <c r="S23" s="26"/>
+      <c r="T23" s="22"/>
+      <c r="U23" s="22"/>
+      <c r="V23" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="W23" s="7"/>
+      <c r="Y23" s="22"/>
+      <c r="Z23" s="22"/>
+      <c r="AA23" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="AB23" s="7"/>
+      <c r="AD23" s="22"/>
+      <c r="AE23" s="22"/>
+      <c r="AF23" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG23" s="7"/>
+    </row>
+    <row r="24" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B24" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C24" s="10"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H24" s="7"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
+      <c r="L24" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="M24" s="7"/>
+      <c r="O24" s="22"/>
+      <c r="P24" s="22"/>
+      <c r="Q24" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="R24" s="7"/>
+      <c r="S24" s="26"/>
+      <c r="T24" s="22"/>
+      <c r="U24" s="22"/>
+      <c r="V24" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="W24" s="7"/>
+    </row>
+    <row r="25" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B25" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="C25" s="10"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="H25" s="7"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="M25" s="7"/>
+      <c r="Q25" s="24"/>
+      <c r="R25" s="24"/>
+      <c r="S25" s="26"/>
+      <c r="T25" s="22"/>
+      <c r="U25" s="22"/>
+      <c r="V25" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="W25" s="7"/>
+    </row>
+    <row r="26" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B26" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="10"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="H26" s="7"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="M26" s="7"/>
+      <c r="Q26" s="24"/>
+      <c r="R26" s="24"/>
+      <c r="S26" s="26"/>
+      <c r="T26" s="26"/>
+    </row>
+    <row r="27" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B27" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="10"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="H27" s="10"/>
+      <c r="Q27" s="24"/>
+      <c r="R27" s="24"/>
+      <c r="S27" s="26"/>
+      <c r="T27" s="26"/>
+    </row>
+    <row r="28" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B28" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="7"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="H28" s="7"/>
+      <c r="J28" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="K28" s="16"/>
+      <c r="L28" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="M28" s="12"/>
+      <c r="O28" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="P28" s="16"/>
+      <c r="Q28" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="R28" s="12"/>
+      <c r="T28" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="U28" s="16"/>
+      <c r="V28" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="W28" s="12"/>
+      <c r="Y28" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="Z28" s="16"/>
+      <c r="AA28" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB28" s="12"/>
+      <c r="AD28" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="AE28" s="16"/>
+      <c r="AF28" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="AG28" s="12"/>
+      <c r="AI28" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="AJ28" s="16"/>
+      <c r="AK28" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="AL28" s="12"/>
+      <c r="AN28" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="AO28" s="16"/>
+      <c r="AP28" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="AQ28" s="12"/>
+    </row>
+    <row r="29" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B29" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="C29" s="7"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H29" s="7"/>
+      <c r="J29" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="K29" s="22"/>
+      <c r="L29" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="M29" s="7"/>
+      <c r="O29" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="P29" s="22"/>
+      <c r="Q29" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="R29" s="7"/>
+      <c r="T29" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="U29" s="22"/>
+      <c r="V29" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="W29" s="7"/>
+      <c r="Y29" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z29" s="22"/>
+      <c r="AA29" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB29" s="7"/>
+      <c r="AD29" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE29" s="22"/>
+      <c r="AF29" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="AG29" s="7"/>
+      <c r="AI29" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="AJ29" s="22"/>
+      <c r="AK29" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="AL29" s="7"/>
+      <c r="AN29" s="22" t="s">
+        <v>193</v>
+      </c>
+      <c r="AO29" s="22"/>
+      <c r="AP29" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="AQ29" s="7"/>
+    </row>
+    <row r="30" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B30" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="C30" s="7"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="H30" s="10"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="22"/>
+      <c r="L30" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="M30" s="7"/>
+      <c r="O30" s="22"/>
+      <c r="P30" s="22"/>
+      <c r="Q30" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="R30" s="7"/>
+      <c r="T30" s="22"/>
+      <c r="U30" s="22"/>
+      <c r="V30" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="W30" s="7"/>
+      <c r="Y30" s="22"/>
+      <c r="Z30" s="22"/>
+      <c r="AA30" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB30" s="7"/>
+      <c r="AD30" s="22"/>
+      <c r="AE30" s="22"/>
+      <c r="AF30" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="AG30" s="7"/>
+      <c r="AI30" s="22"/>
+      <c r="AJ30" s="22"/>
+      <c r="AK30" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AL30" s="7"/>
+      <c r="AN30" s="22"/>
+      <c r="AO30" s="22"/>
+      <c r="AP30" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="AQ30" s="7"/>
+    </row>
+    <row r="31" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B31" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="C31" s="7"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="H31" s="7"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
+      <c r="L31" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="M31" s="7"/>
+      <c r="O31" s="22"/>
+      <c r="P31" s="22"/>
+      <c r="Q31" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="R31" s="7"/>
+      <c r="T31" s="22"/>
+      <c r="U31" s="22"/>
+      <c r="V31" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="W31" s="7"/>
+      <c r="Y31" s="22"/>
+      <c r="Z31" s="22"/>
+      <c r="AA31" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB31" s="7"/>
+      <c r="AD31" s="22"/>
+      <c r="AE31" s="22"/>
+      <c r="AF31" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="AG31" s="7"/>
+      <c r="AI31" s="22"/>
+      <c r="AJ31" s="22"/>
+      <c r="AK31" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="AL31" s="7"/>
+      <c r="AN31" s="22"/>
+      <c r="AO31" s="22"/>
+      <c r="AP31" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="AQ31" s="7"/>
+    </row>
+    <row r="32" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B32" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="7"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="22"/>
+      <c r="L32" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="M32" s="7"/>
+      <c r="O32" s="22"/>
+      <c r="P32" s="22"/>
+      <c r="Q32" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="R32" s="7"/>
+      <c r="T32" s="22"/>
+      <c r="U32" s="22"/>
+      <c r="V32" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="W32" s="7"/>
+      <c r="Y32" s="22"/>
+      <c r="Z32" s="22"/>
+      <c r="AA32" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="AB32" s="7"/>
+      <c r="AD32" s="22"/>
+      <c r="AE32" s="22"/>
+      <c r="AF32" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="AG32" s="7"/>
+      <c r="AI32" s="22"/>
+      <c r="AJ32" s="22"/>
+      <c r="AK32" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="AL32" s="7"/>
+      <c r="AN32" s="22"/>
+      <c r="AO32" s="22"/>
+      <c r="AP32" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="AQ32" s="7"/>
+    </row>
+    <row r="33" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B33" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33" s="7"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="22"/>
+      <c r="L33" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="M33" s="7"/>
+      <c r="O33" s="22"/>
+      <c r="P33" s="22"/>
+      <c r="Q33" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="R33" s="7"/>
+      <c r="T33" s="22"/>
+      <c r="U33" s="22"/>
+      <c r="V33" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="W33" s="22"/>
+      <c r="Y33" s="22"/>
+      <c r="Z33" s="22"/>
+      <c r="AA33" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB33" s="7"/>
+      <c r="AD33" s="22"/>
+      <c r="AE33" s="22"/>
+      <c r="AF33" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="AG33" s="7"/>
+      <c r="AI33" s="22"/>
+      <c r="AJ33" s="22"/>
+      <c r="AK33" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="AL33" s="7"/>
+      <c r="AN33" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="AO33" s="22"/>
+      <c r="AP33" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="AQ33" s="7"/>
+    </row>
+    <row r="34" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="22"/>
+      <c r="L34" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="M34" s="7"/>
+      <c r="O34" s="22"/>
+      <c r="P34" s="22"/>
+      <c r="Q34" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="R34" s="7"/>
+      <c r="Y34" s="22"/>
+      <c r="Z34" s="22"/>
+      <c r="AA34" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB34" s="7"/>
+      <c r="AD34" s="22"/>
+      <c r="AE34" s="22"/>
+      <c r="AF34" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="AG34" s="7"/>
+      <c r="AI34" s="22"/>
+      <c r="AJ34" s="22"/>
+      <c r="AK34" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="AL34" s="7"/>
+      <c r="AN34" s="22"/>
+      <c r="AO34" s="22"/>
+      <c r="AP34" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="AQ34" s="7"/>
+    </row>
+    <row r="35" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22"/>
+      <c r="L35" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="M35" s="7"/>
+      <c r="O35" s="22"/>
+      <c r="P35" s="22"/>
+      <c r="Q35" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="R35" s="7"/>
+      <c r="T35" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="U35" s="16"/>
+      <c r="V35" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="W35" s="12"/>
+      <c r="Y35" s="22"/>
+      <c r="Z35" s="22"/>
+      <c r="AA35" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB35" s="7"/>
+      <c r="AD35" s="22"/>
+      <c r="AE35" s="22"/>
+      <c r="AF35" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="AG35" s="7"/>
+      <c r="AI35" s="22"/>
+      <c r="AJ35" s="22"/>
+      <c r="AK35" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="AL35" s="7"/>
+      <c r="AN35" s="22"/>
+      <c r="AO35" s="22"/>
+      <c r="AP35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AQ35" s="7"/>
+    </row>
+    <row r="36" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
+      <c r="O36" s="22"/>
+      <c r="P36" s="22"/>
+      <c r="Q36" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="R36" s="7"/>
+      <c r="T36" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="U36" s="7"/>
+      <c r="V36" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="W36" s="7"/>
+      <c r="Y36" s="22"/>
+      <c r="Z36" s="22"/>
+      <c r="AA36" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="AB36" s="7"/>
+      <c r="AD36" s="22"/>
+      <c r="AE36" s="22"/>
+      <c r="AF36" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG36" s="7"/>
+      <c r="AI36" s="22"/>
+      <c r="AJ36" s="22"/>
+      <c r="AK36" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL36" s="7"/>
+      <c r="AN36" s="22"/>
+      <c r="AO36" s="22"/>
+      <c r="AP36" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="AQ36" s="7"/>
+    </row>
+    <row r="37" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="D37" s="26"/>
+      <c r="E37" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="F37" s="16"/>
+      <c r="G37" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="H37" s="12"/>
+      <c r="J37" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="K37" s="16"/>
+      <c r="L37" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="M37" s="12"/>
+      <c r="O37" s="22"/>
+      <c r="P37" s="22"/>
+      <c r="Q37" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="R37" s="7"/>
+      <c r="S37" s="26"/>
+      <c r="T37" s="26"/>
+      <c r="Y37" s="22"/>
+      <c r="Z37" s="22"/>
+      <c r="AA37" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="AB37" s="7"/>
+      <c r="AN37" s="22"/>
+      <c r="AO37" s="22"/>
+      <c r="AP37" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="AQ37" s="7"/>
+    </row>
+    <row r="38" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B38" s="26"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="F38" s="22"/>
+      <c r="G38" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="H38" s="7"/>
+      <c r="J38" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="K38" s="22"/>
+      <c r="L38" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="M38" s="7"/>
+      <c r="Q38" s="26"/>
+      <c r="R38" s="26"/>
+      <c r="S38" s="26"/>
+      <c r="T38" s="26"/>
+      <c r="Y38" s="22"/>
+      <c r="Z38" s="22"/>
+      <c r="AA38" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="AB38" s="7"/>
+      <c r="AN38" s="22"/>
+      <c r="AO38" s="22"/>
+      <c r="AP38" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="AQ38" s="7"/>
+    </row>
+    <row r="39" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B39" s="26"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="H39" s="7"/>
+      <c r="J39" s="22"/>
+      <c r="K39" s="22"/>
+      <c r="L39" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M39" s="7"/>
+      <c r="Q39" s="26"/>
+      <c r="R39" s="26"/>
+      <c r="S39" s="26"/>
+      <c r="T39" s="26"/>
+      <c r="Y39" s="22"/>
+      <c r="Z39" s="22"/>
+      <c r="AA39" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB39" s="7"/>
+    </row>
+    <row r="40" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B40" s="28"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="H40" s="7"/>
+      <c r="J40" s="22"/>
+      <c r="K40" s="22"/>
+      <c r="L40" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="M40" s="7"/>
+      <c r="Q40" s="26"/>
+      <c r="R40" s="26"/>
+      <c r="S40" s="26"/>
+      <c r="T40" s="26"/>
+      <c r="Y40" s="22"/>
+      <c r="Z40" s="22"/>
+      <c r="AA40" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="AB40" s="7"/>
+    </row>
+    <row r="41" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="H41" s="7"/>
+      <c r="J41" s="22"/>
+      <c r="K41" s="22"/>
+      <c r="L41" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="M41" s="7"/>
+      <c r="Q41" s="26"/>
+      <c r="R41" s="26"/>
+      <c r="S41" s="26"/>
+      <c r="T41" s="26"/>
+      <c r="Y41" s="22"/>
+      <c r="Z41" s="22"/>
+      <c r="AA41" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="AB41" s="7"/>
+    </row>
+    <row r="42" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B42" s="26"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="Q42" s="26"/>
+      <c r="R42" s="26"/>
+      <c r="S42" s="26"/>
+      <c r="T42" s="26"/>
+      <c r="Y42" s="22"/>
+      <c r="Z42" s="22"/>
+      <c r="AA42" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB42" s="7"/>
+    </row>
+    <row r="43" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B43" s="26"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
+      <c r="Q43" s="26"/>
+      <c r="R43" s="26"/>
+      <c r="S43" s="26"/>
+      <c r="T43" s="26"/>
+    </row>
+    <row r="44" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B44" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C44" s="8"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="26"/>
+      <c r="Q44" s="26"/>
+      <c r="R44" s="26"/>
+      <c r="S44" s="26"/>
+      <c r="T44" s="26"/>
+    </row>
+    <row r="45" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B45" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C45" s="7"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="27"/>
+      <c r="Q45" s="27"/>
+      <c r="R45" s="27"/>
+      <c r="S45" s="27"/>
+      <c r="T45" s="27"/>
+    </row>
+    <row r="46" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B46" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C46" s="7"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="27"/>
+      <c r="Q46" s="27"/>
+      <c r="R46" s="27"/>
+      <c r="S46" s="27"/>
+      <c r="T46" s="27"/>
+    </row>
+    <row r="47" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B47" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C47" s="7"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
+      <c r="Q47" s="26"/>
+      <c r="R47" s="26"/>
+      <c r="S47" s="26"/>
+      <c r="T47" s="26"/>
+    </row>
+    <row r="48" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B48" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C48" s="7"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="27"/>
+      <c r="Q48" s="27"/>
+      <c r="R48" s="27"/>
+      <c r="S48" s="27"/>
+      <c r="T48" s="27"/>
+    </row>
+    <row r="49" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B49" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C49" s="7"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="24"/>
+      <c r="Q49" s="24"/>
+      <c r="R49" s="24"/>
+      <c r="S49" s="24"/>
+      <c r="T49" s="24"/>
+    </row>
+    <row r="50" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B50" s="26"/>
+      <c r="C50" s="26"/>
+      <c r="D50" s="24"/>
+      <c r="E50" s="24"/>
+      <c r="Q50" s="24"/>
+      <c r="R50" s="24"/>
+      <c r="S50" s="24"/>
+      <c r="T50" s="24"/>
+    </row>
+    <row r="51" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B51" s="28"/>
+      <c r="C51" s="28"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="24"/>
+      <c r="Q51" s="24"/>
+      <c r="R51" s="24"/>
+      <c r="S51" s="24"/>
+      <c r="T51" s="24"/>
+    </row>
+    <row r="52" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B52" s="24"/>
+      <c r="C52" s="24"/>
+      <c r="D52" s="24"/>
+      <c r="E52" s="24"/>
+      <c r="Q52" s="28"/>
+      <c r="R52" s="28"/>
+      <c r="S52" s="24"/>
+      <c r="T52" s="24"/>
+    </row>
+    <row r="53" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B53" s="24"/>
+      <c r="C53" s="24"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="24"/>
+    </row>
+    <row r="54" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B54" s="24"/>
+      <c r="C54" s="24"/>
+      <c r="D54" s="24"/>
+      <c r="E54" s="24"/>
+    </row>
+    <row r="55" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B55" s="24"/>
+      <c r="C55" s="24"/>
+      <c r="D55" s="24"/>
+      <c r="E55" s="24"/>
+    </row>
+    <row r="56" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B56" s="24"/>
+      <c r="C56" s="24"/>
+      <c r="D56" s="24"/>
+      <c r="E56" s="24"/>
+    </row>
+    <row r="57" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B57" s="24"/>
+      <c r="C57" s="24"/>
+      <c r="D57" s="24"/>
+      <c r="E57" s="24"/>
+    </row>
+    <row r="58" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B58" s="27"/>
+      <c r="C58" s="27"/>
+      <c r="D58" s="27"/>
+      <c r="E58" s="27"/>
+    </row>
+    <row r="59" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B59" s="24"/>
+      <c r="C59" s="24"/>
+      <c r="D59" s="24"/>
+      <c r="E59" s="24"/>
+    </row>
+    <row r="60" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B60" s="24"/>
+      <c r="C60" s="24"/>
+      <c r="D60" s="24"/>
+      <c r="E60" s="24"/>
+    </row>
+    <row r="61" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B61" s="28"/>
+      <c r="C61" s="28"/>
+      <c r="D61" s="24"/>
+      <c r="E61" s="24"/>
+    </row>
+    <row r="62" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B62" s="28"/>
+      <c r="C62" s="28"/>
+      <c r="D62" s="27"/>
+      <c r="E62" s="27"/>
+    </row>
+    <row r="63" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B63" s="28"/>
+      <c r="C63" s="28"/>
+      <c r="D63" s="27"/>
+      <c r="E63" s="27"/>
+    </row>
+    <row r="154" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H154" s="21"/>
+      <c r="I154" s="21"/>
+      <c r="J154" s="21"/>
+      <c r="K154" s="21"/>
+    </row>
+    <row r="191" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J191" s="21"/>
+      <c r="K191" s="21"/>
+    </row>
+  </sheetData>
+  <mergeCells count="343">
+    <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AJ4:AK4"/>
+    <mergeCell ref="AJ5:AK5"/>
+    <mergeCell ref="AJ6:AK6"/>
+    <mergeCell ref="AJ7:AK7"/>
+    <mergeCell ref="AL4:AM4"/>
+    <mergeCell ref="AL5:AM5"/>
+    <mergeCell ref="AL6:AM6"/>
+    <mergeCell ref="AL7:AM7"/>
+    <mergeCell ref="AG6:AH6"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="T12:U12"/>
+    <mergeCell ref="V12:W12"/>
+    <mergeCell ref="Y12:Z12"/>
+    <mergeCell ref="AA12:AB12"/>
+    <mergeCell ref="AD12:AE12"/>
+    <mergeCell ref="AF12:AG12"/>
+    <mergeCell ref="AI12:AJ12"/>
+    <mergeCell ref="AK12:AL12"/>
+    <mergeCell ref="AN12:AO12"/>
+    <mergeCell ref="AP12:AQ12"/>
+    <mergeCell ref="V4:Y4"/>
+    <mergeCell ref="V5:Y5"/>
+    <mergeCell ref="V6:Y6"/>
+    <mergeCell ref="V7:Y7"/>
+    <mergeCell ref="V8:Y8"/>
+    <mergeCell ref="AP36:AQ36"/>
+    <mergeCell ref="AP37:AQ37"/>
+    <mergeCell ref="J191:K191"/>
+    <mergeCell ref="AP29:AQ29"/>
+    <mergeCell ref="AP30:AQ30"/>
+    <mergeCell ref="AP31:AQ31"/>
+    <mergeCell ref="AP32:AQ32"/>
+    <mergeCell ref="AN29:AO32"/>
+    <mergeCell ref="AP33:AQ33"/>
+    <mergeCell ref="AP34:AQ34"/>
+    <mergeCell ref="AP35:AQ35"/>
+    <mergeCell ref="AP38:AQ38"/>
+    <mergeCell ref="AN33:AO38"/>
+    <mergeCell ref="AF36:AG36"/>
+    <mergeCell ref="AD29:AE36"/>
+    <mergeCell ref="AP18:AQ18"/>
+    <mergeCell ref="AP15:AQ15"/>
+    <mergeCell ref="AP20:AQ20"/>
+    <mergeCell ref="AN13:AO20"/>
+    <mergeCell ref="AP17:AQ17"/>
+    <mergeCell ref="AP16:AQ16"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="E38:F41"/>
+    <mergeCell ref="AP19:AQ19"/>
+    <mergeCell ref="AN28:AO28"/>
+    <mergeCell ref="AP28:AQ28"/>
+    <mergeCell ref="T13:U25"/>
+    <mergeCell ref="AA23:AB23"/>
+    <mergeCell ref="Y13:Z23"/>
+    <mergeCell ref="AK21:AL21"/>
+    <mergeCell ref="AI13:AJ21"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="AI29:AJ36"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="O29:P37"/>
+    <mergeCell ref="AP13:AQ13"/>
+    <mergeCell ref="AP14:AQ14"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="L37:M37"/>
+    <mergeCell ref="AK31:AL31"/>
+    <mergeCell ref="AK32:AL32"/>
+    <mergeCell ref="AK34:AL34"/>
+    <mergeCell ref="AK33:AL33"/>
+    <mergeCell ref="AK35:AL35"/>
+    <mergeCell ref="AK36:AL36"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="AF31:AG31"/>
+    <mergeCell ref="AF30:AG30"/>
+    <mergeCell ref="AF32:AG32"/>
+    <mergeCell ref="AF33:AG33"/>
+    <mergeCell ref="AF34:AG34"/>
+    <mergeCell ref="AF35:AG35"/>
+    <mergeCell ref="AK29:AL29"/>
+    <mergeCell ref="AK30:AL30"/>
+    <mergeCell ref="AA42:AB42"/>
+    <mergeCell ref="Y29:Z42"/>
+    <mergeCell ref="L38:M38"/>
+    <mergeCell ref="L39:M39"/>
+    <mergeCell ref="L40:M40"/>
+    <mergeCell ref="L41:M41"/>
+    <mergeCell ref="J154:K154"/>
+    <mergeCell ref="AF29:AG29"/>
+    <mergeCell ref="J38:K41"/>
+    <mergeCell ref="H154:I154"/>
+    <mergeCell ref="T35:U35"/>
+    <mergeCell ref="V35:W35"/>
+    <mergeCell ref="T36:U36"/>
+    <mergeCell ref="V36:W36"/>
+    <mergeCell ref="AA35:AB35"/>
+    <mergeCell ref="AA36:AB36"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="AA37:AB37"/>
+    <mergeCell ref="AA38:AB38"/>
+    <mergeCell ref="AA39:AB39"/>
+    <mergeCell ref="AA40:AB40"/>
+    <mergeCell ref="AA41:AB41"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="Y28:Z28"/>
+    <mergeCell ref="AA28:AB28"/>
+    <mergeCell ref="AA29:AB29"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="AA30:AB30"/>
+    <mergeCell ref="AA31:AB31"/>
+    <mergeCell ref="AA32:AB32"/>
+    <mergeCell ref="AA33:AB33"/>
+    <mergeCell ref="AA34:AB34"/>
+    <mergeCell ref="Q31:R31"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="Q35:R35"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="Q37:R37"/>
+    <mergeCell ref="T29:U33"/>
+    <mergeCell ref="V29:W29"/>
+    <mergeCell ref="V32:W32"/>
+    <mergeCell ref="V33:W33"/>
+    <mergeCell ref="V31:W31"/>
+    <mergeCell ref="V30:W30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="L35:M35"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="J29:K35"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="AF19:AG19"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="AK16:AL16"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="J23:K26"/>
+    <mergeCell ref="T28:U28"/>
+    <mergeCell ref="V28:W28"/>
+    <mergeCell ref="AD28:AE28"/>
+    <mergeCell ref="AF28:AG28"/>
+    <mergeCell ref="AI28:AJ28"/>
+    <mergeCell ref="AK28:AL28"/>
+    <mergeCell ref="AK13:AL13"/>
+    <mergeCell ref="AK15:AL15"/>
+    <mergeCell ref="AK17:AL17"/>
+    <mergeCell ref="AK18:AL18"/>
+    <mergeCell ref="AK14:AL14"/>
+    <mergeCell ref="AK19:AL19"/>
+    <mergeCell ref="AK20:AL20"/>
+    <mergeCell ref="AF17:AG17"/>
+    <mergeCell ref="AF18:AG18"/>
+    <mergeCell ref="AF20:AG20"/>
+    <mergeCell ref="AF21:AG21"/>
+    <mergeCell ref="AF22:AG22"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="O13:P24"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="AD13:AE23"/>
+    <mergeCell ref="AF23:AG23"/>
+    <mergeCell ref="AA20:AB20"/>
+    <mergeCell ref="AA21:AB21"/>
+    <mergeCell ref="AA22:AB22"/>
+    <mergeCell ref="AF13:AG13"/>
+    <mergeCell ref="AF14:AG14"/>
+    <mergeCell ref="AF15:AG15"/>
+    <mergeCell ref="AF16:AG16"/>
+    <mergeCell ref="V25:W25"/>
+    <mergeCell ref="AA13:AB13"/>
+    <mergeCell ref="AA14:AB14"/>
+    <mergeCell ref="AA15:AB15"/>
+    <mergeCell ref="AA16:AB16"/>
+    <mergeCell ref="AA17:AB17"/>
+    <mergeCell ref="AA18:AB18"/>
+    <mergeCell ref="AA19:AB19"/>
+    <mergeCell ref="V18:W18"/>
+    <mergeCell ref="V19:W19"/>
+    <mergeCell ref="V20:W20"/>
+    <mergeCell ref="V21:W21"/>
+    <mergeCell ref="V22:W22"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="V24:W24"/>
+    <mergeCell ref="V14:W14"/>
+    <mergeCell ref="V15:W15"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="V13:W13"/>
+    <mergeCell ref="V16:W16"/>
+    <mergeCell ref="V17:W17"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="Q16:R16"/>
+    <mergeCell ref="J13:K20"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="E13:F31"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="AA4:AB4"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AA6:AB6"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="O4:R4"/>
+    <mergeCell ref="O5:R5"/>
+    <mergeCell ref="O6:R6"/>
+    <mergeCell ref="O7:R7"/>
+    <mergeCell ref="O8:R8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="T7:U7"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="T8:U8"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="Q49:R49"/>
+    <mergeCell ref="Q50:R50"/>
+    <mergeCell ref="Q51:R51"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="S49:T49"/>
+    <mergeCell ref="S50:T50"/>
+    <mergeCell ref="S51:T51"/>
+    <mergeCell ref="S52:T52"/>
+    <mergeCell ref="AA7:AB7"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="B30:C30"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -946,9 +3922,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Change data in object
</commit_message>
<xml_diff>
--- a/Doccuments/Object/ObjectInfo.xlsx
+++ b/Doccuments/Object/ObjectInfo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="96" windowWidth="12420" windowHeight="5856"/>
+    <workbookView xWindow="480" yWindow="96" windowWidth="12420" windowHeight="5856" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CSDL" sheetId="2" r:id="rId1"/>
@@ -654,10 +654,10 @@
     <t>Thu/Chi</t>
   </si>
   <si>
-    <t>Object</t>
-  </si>
-  <si>
     <t>Gia đình nằm trong nhóm</t>
+  </si>
+  <si>
+    <t>HashMap&lt;ID, Object Nhóm&gt;</t>
   </si>
 </sst>
 </file>
@@ -803,7 +803,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -1310,11 +1310,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1342,164 +1355,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1509,25 +1369,181 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1920,7 +1936,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:AQ191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="G24" sqref="G24:H24"/>
     </sheetView>
   </sheetViews>
@@ -1940,258 +1956,258 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="55" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="H4" s="30"/>
-      <c r="I4" s="24" t="s">
+      <c r="H4" s="59"/>
+      <c r="I4" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="M4" s="25" t="s">
+      <c r="J4" s="55"/>
+      <c r="K4" s="55"/>
+      <c r="M4" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="N4" s="25"/>
-      <c r="O4" s="24" t="s">
+      <c r="N4" s="61"/>
+      <c r="O4" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="24"/>
-      <c r="AA4" s="23" t="s">
+      <c r="P4" s="55"/>
+      <c r="Q4" s="55"/>
+      <c r="R4" s="55"/>
+      <c r="AA4" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="AB4" s="23"/>
+      <c r="AB4" s="60"/>
       <c r="AC4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AE4" s="31" t="s">
+      <c r="AE4" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="AF4" s="31"/>
-      <c r="AG4" s="16" t="s">
+      <c r="AF4" s="35"/>
+      <c r="AG4" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="AH4" s="16"/>
-      <c r="AJ4" s="43" t="s">
+      <c r="AH4" s="37"/>
+      <c r="AJ4" s="36" t="s">
         <v>205</v>
       </c>
-      <c r="AK4" s="43"/>
-      <c r="AL4" s="16" t="s">
+      <c r="AK4" s="36"/>
+      <c r="AL4" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="AM4" s="16"/>
+      <c r="AM4" s="37"/>
     </row>
     <row r="5" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
       <c r="E5" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16" t="s">
+      <c r="H5" s="37"/>
+      <c r="I5" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="M5" s="26" t="s">
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="M5" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="N5" s="26"/>
-      <c r="O5" s="16" t="s">
+      <c r="N5" s="62"/>
+      <c r="O5" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="16"/>
-      <c r="AA5" s="16" t="s">
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="37"/>
+      <c r="AA5" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="AB5" s="16"/>
+      <c r="AB5" s="37"/>
       <c r="AC5" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AE5" s="43" t="s">
+      <c r="AE5" s="36" t="s">
         <v>205</v>
       </c>
-      <c r="AF5" s="43"/>
-      <c r="AG5" s="16" t="s">
+      <c r="AF5" s="36"/>
+      <c r="AG5" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="AH5" s="16"/>
-      <c r="AJ5" s="16" t="s">
+      <c r="AH5" s="37"/>
+      <c r="AJ5" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="AK5" s="16"/>
-      <c r="AL5" s="16" t="s">
+      <c r="AK5" s="37"/>
+      <c r="AL5" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="AM5" s="16"/>
+      <c r="AM5" s="37"/>
     </row>
     <row r="6" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="57" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
       <c r="E6" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16" t="s">
+      <c r="H6" s="37"/>
+      <c r="I6" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="M6" s="16" t="s">
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="M6" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16" t="s">
+      <c r="N6" s="37"/>
+      <c r="O6" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="16"/>
-      <c r="AA6" s="16" t="s">
+      <c r="P6" s="37"/>
+      <c r="Q6" s="37"/>
+      <c r="R6" s="37"/>
+      <c r="AA6" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="AB6" s="16"/>
+      <c r="AB6" s="37"/>
       <c r="AC6" s="3" t="s">
         <v>204</v>
       </c>
       <c r="AE6" s="7"/>
       <c r="AF6" s="7"/>
-      <c r="AG6" s="44"/>
-      <c r="AH6" s="44"/>
-      <c r="AJ6" s="16" t="s">
+      <c r="AG6" s="38"/>
+      <c r="AH6" s="38"/>
+      <c r="AJ6" s="37" t="s">
         <v>200</v>
       </c>
-      <c r="AK6" s="16"/>
-      <c r="AL6" s="16" t="s">
+      <c r="AK6" s="37"/>
+      <c r="AL6" s="37" t="s">
         <v>203</v>
       </c>
-      <c r="AM6" s="16"/>
+      <c r="AM6" s="37"/>
     </row>
     <row r="7" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="58" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
       <c r="E7" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17" t="s">
+      <c r="H7" s="43"/>
+      <c r="I7" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="M7" s="16" t="s">
+      <c r="J7" s="43"/>
+      <c r="K7" s="43"/>
+      <c r="M7" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16" t="s">
+      <c r="N7" s="37"/>
+      <c r="O7" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="16"/>
-      <c r="AA7" s="16" t="s">
+      <c r="P7" s="37"/>
+      <c r="Q7" s="37"/>
+      <c r="R7" s="37"/>
+      <c r="AA7" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="AB7" s="16"/>
+      <c r="AB7" s="37"/>
       <c r="AC7" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AJ7" s="16" t="s">
+      <c r="AJ7" s="37" t="s">
         <v>201</v>
       </c>
-      <c r="AK7" s="16"/>
-      <c r="AL7" s="16" t="s">
+      <c r="AK7" s="37"/>
+      <c r="AL7" s="37" t="s">
         <v>202</v>
       </c>
-      <c r="AM7" s="16"/>
+      <c r="AM7" s="37"/>
     </row>
     <row r="8" spans="2:43" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
       <c r="E8" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17" t="s">
+      <c r="H8" s="43"/>
+      <c r="I8" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="M8" s="16" t="s">
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="M8" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16" t="s">
+      <c r="N8" s="37"/>
+      <c r="O8" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="16"/>
+      <c r="P8" s="37"/>
+      <c r="Q8" s="37"/>
+      <c r="R8" s="37"/>
     </row>
     <row r="9" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
       <c r="E9" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16" t="s">
+      <c r="H9" s="37"/>
+      <c r="I9" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="Q9" s="21"/>
-      <c r="R9" s="21"/>
-      <c r="S9" s="21"/>
-      <c r="T9" s="21"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="Q9" s="63"/>
+      <c r="R9" s="63"/>
+      <c r="S9" s="63"/>
+      <c r="T9" s="63"/>
     </row>
     <row r="10" spans="2:43" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="Q10" s="15"/>
-      <c r="R10" s="15"/>
-      <c r="S10" s="15"/>
-      <c r="T10" s="15"/>
+      <c r="Q10" s="53"/>
+      <c r="R10" s="53"/>
+      <c r="S10" s="53"/>
+      <c r="T10" s="53"/>
     </row>
     <row r="11" spans="2:43" ht="16.5" x14ac:dyDescent="0.25">
       <c r="Q11" s="9"/>
@@ -2200,1402 +2216,1402 @@
       <c r="T11" s="9"/>
     </row>
     <row r="12" spans="2:43" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="E12" s="17" t="s">
+      <c r="C12" s="42"/>
+      <c r="E12" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="F12" s="17"/>
-      <c r="G12" s="22" t="s">
+      <c r="F12" s="43"/>
+      <c r="G12" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="H12" s="22"/>
-      <c r="J12" s="17" t="s">
+      <c r="H12" s="44"/>
+      <c r="J12" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="K12" s="17"/>
-      <c r="L12" s="22" t="s">
+      <c r="K12" s="43"/>
+      <c r="L12" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="M12" s="22"/>
-      <c r="O12" s="17" t="s">
+      <c r="M12" s="44"/>
+      <c r="O12" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="P12" s="17"/>
-      <c r="Q12" s="22" t="s">
+      <c r="P12" s="43"/>
+      <c r="Q12" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="R12" s="22"/>
+      <c r="R12" s="44"/>
       <c r="S12" s="9"/>
-      <c r="T12" s="17" t="s">
+      <c r="T12" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="U12" s="17"/>
-      <c r="V12" s="22" t="s">
+      <c r="U12" s="43"/>
+      <c r="V12" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="W12" s="22"/>
-      <c r="Y12" s="17" t="s">
+      <c r="W12" s="44"/>
+      <c r="Y12" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="Z12" s="17"/>
-      <c r="AA12" s="22" t="s">
+      <c r="Z12" s="43"/>
+      <c r="AA12" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="AB12" s="22"/>
-      <c r="AD12" s="17" t="s">
+      <c r="AB12" s="44"/>
+      <c r="AD12" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="AE12" s="17"/>
-      <c r="AF12" s="22" t="s">
+      <c r="AE12" s="43"/>
+      <c r="AF12" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="AG12" s="22"/>
-      <c r="AI12" s="17" t="s">
+      <c r="AG12" s="44"/>
+      <c r="AI12" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="AJ12" s="17"/>
-      <c r="AK12" s="22" t="s">
+      <c r="AJ12" s="43"/>
+      <c r="AK12" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="AL12" s="22"/>
-      <c r="AN12" s="17" t="s">
+      <c r="AL12" s="44"/>
+      <c r="AN12" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="AO12" s="17"/>
-      <c r="AP12" s="22" t="s">
+      <c r="AO12" s="43"/>
+      <c r="AP12" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="AQ12" s="22"/>
+      <c r="AQ12" s="44"/>
     </row>
     <row r="13" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="20"/>
-      <c r="E13" s="37" t="s">
+      <c r="C13" s="40"/>
+      <c r="E13" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="F13" s="38"/>
-      <c r="G13" s="16" t="s">
+      <c r="F13" s="47"/>
+      <c r="G13" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="H13" s="16"/>
-      <c r="J13" s="32" t="s">
+      <c r="H13" s="37"/>
+      <c r="J13" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="K13" s="32"/>
-      <c r="L13" s="16" t="s">
+      <c r="K13" s="45"/>
+      <c r="L13" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="M13" s="16"/>
-      <c r="O13" s="32" t="s">
+      <c r="M13" s="37"/>
+      <c r="O13" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="P13" s="32"/>
-      <c r="Q13" s="16" t="s">
+      <c r="P13" s="45"/>
+      <c r="Q13" s="37" t="s">
         <v>130</v>
       </c>
-      <c r="R13" s="16"/>
+      <c r="R13" s="37"/>
       <c r="S13" s="9"/>
-      <c r="T13" s="32" t="s">
+      <c r="T13" s="45" t="s">
         <v>106</v>
       </c>
-      <c r="U13" s="32"/>
-      <c r="V13" s="16" t="s">
+      <c r="U13" s="45"/>
+      <c r="V13" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="W13" s="16"/>
-      <c r="Y13" s="32" t="s">
+      <c r="W13" s="37"/>
+      <c r="Y13" s="45" t="s">
         <v>123</v>
       </c>
-      <c r="Z13" s="32"/>
-      <c r="AA13" s="16" t="s">
+      <c r="Z13" s="45"/>
+      <c r="AA13" s="37" t="s">
         <v>118</v>
       </c>
-      <c r="AB13" s="16"/>
-      <c r="AD13" s="32" t="s">
+      <c r="AB13" s="37"/>
+      <c r="AD13" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="AE13" s="32"/>
-      <c r="AF13" s="16" t="s">
+      <c r="AE13" s="45"/>
+      <c r="AF13" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="AG13" s="16"/>
-      <c r="AI13" s="32" t="s">
+      <c r="AG13" s="37"/>
+      <c r="AI13" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="AJ13" s="32"/>
-      <c r="AK13" s="16" t="s">
+      <c r="AJ13" s="45"/>
+      <c r="AK13" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="AL13" s="16"/>
-      <c r="AN13" s="32" t="s">
+      <c r="AL13" s="37"/>
+      <c r="AN13" s="45" t="s">
         <v>187</v>
       </c>
-      <c r="AO13" s="32"/>
-      <c r="AP13" s="16" t="s">
+      <c r="AO13" s="45"/>
+      <c r="AP13" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="AQ13" s="16"/>
+      <c r="AQ13" s="37"/>
     </row>
     <row r="14" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="C14" s="20"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="16" t="s">
+      <c r="C14" s="40"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="H14" s="16"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="32"/>
-      <c r="L14" s="16" t="s">
+      <c r="H14" s="37"/>
+      <c r="J14" s="45"/>
+      <c r="K14" s="45"/>
+      <c r="L14" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="M14" s="16"/>
-      <c r="O14" s="32"/>
-      <c r="P14" s="32"/>
-      <c r="Q14" s="16" t="s">
+      <c r="M14" s="37"/>
+      <c r="O14" s="45"/>
+      <c r="P14" s="45"/>
+      <c r="Q14" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="R14" s="16"/>
+      <c r="R14" s="37"/>
       <c r="S14" s="9"/>
-      <c r="T14" s="32"/>
-      <c r="U14" s="32"/>
-      <c r="V14" s="16" t="s">
+      <c r="T14" s="45"/>
+      <c r="U14" s="45"/>
+      <c r="V14" s="37" t="s">
         <v>116</v>
       </c>
-      <c r="W14" s="16"/>
-      <c r="Y14" s="32"/>
-      <c r="Z14" s="32"/>
-      <c r="AA14" s="16" t="s">
+      <c r="W14" s="37"/>
+      <c r="Y14" s="45"/>
+      <c r="Z14" s="45"/>
+      <c r="AA14" s="37" t="s">
         <v>119</v>
       </c>
-      <c r="AB14" s="16"/>
-      <c r="AD14" s="32"/>
-      <c r="AE14" s="32"/>
-      <c r="AF14" s="16" t="s">
+      <c r="AB14" s="37"/>
+      <c r="AD14" s="45"/>
+      <c r="AE14" s="45"/>
+      <c r="AF14" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="AG14" s="16"/>
-      <c r="AI14" s="32"/>
-      <c r="AJ14" s="32"/>
-      <c r="AK14" s="16" t="s">
+      <c r="AG14" s="37"/>
+      <c r="AI14" s="45"/>
+      <c r="AJ14" s="45"/>
+      <c r="AK14" s="37" t="s">
         <v>142</v>
       </c>
-      <c r="AL14" s="16"/>
-      <c r="AN14" s="32"/>
-      <c r="AO14" s="32"/>
-      <c r="AP14" s="16" t="s">
+      <c r="AL14" s="37"/>
+      <c r="AN14" s="45"/>
+      <c r="AO14" s="45"/>
+      <c r="AP14" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="AQ14" s="16"/>
+      <c r="AQ14" s="37"/>
     </row>
     <row r="15" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="16" t="s">
+      <c r="C15" s="40"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="H15" s="16"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="16" t="s">
+      <c r="H15" s="37"/>
+      <c r="J15" s="45"/>
+      <c r="K15" s="45"/>
+      <c r="L15" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="M15" s="16"/>
-      <c r="O15" s="32"/>
-      <c r="P15" s="32"/>
-      <c r="Q15" s="16" t="s">
+      <c r="M15" s="37"/>
+      <c r="O15" s="45"/>
+      <c r="P15" s="45"/>
+      <c r="Q15" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="R15" s="16"/>
+      <c r="R15" s="37"/>
       <c r="S15" s="9"/>
-      <c r="T15" s="32"/>
-      <c r="U15" s="32"/>
-      <c r="V15" s="16" t="s">
+      <c r="T15" s="45"/>
+      <c r="U15" s="45"/>
+      <c r="V15" s="37" t="s">
         <v>117</v>
       </c>
-      <c r="W15" s="16"/>
-      <c r="Y15" s="32"/>
-      <c r="Z15" s="32"/>
-      <c r="AA15" s="16" t="s">
+      <c r="W15" s="37"/>
+      <c r="Y15" s="45"/>
+      <c r="Z15" s="45"/>
+      <c r="AA15" s="37" t="s">
         <v>120</v>
       </c>
-      <c r="AB15" s="16"/>
-      <c r="AD15" s="32"/>
-      <c r="AE15" s="32"/>
-      <c r="AF15" s="16" t="s">
+      <c r="AB15" s="37"/>
+      <c r="AD15" s="45"/>
+      <c r="AE15" s="45"/>
+      <c r="AF15" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="AG15" s="16"/>
-      <c r="AI15" s="32"/>
-      <c r="AJ15" s="32"/>
-      <c r="AK15" s="16" t="s">
+      <c r="AG15" s="37"/>
+      <c r="AI15" s="45"/>
+      <c r="AJ15" s="45"/>
+      <c r="AK15" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="AL15" s="16"/>
-      <c r="AN15" s="32"/>
-      <c r="AO15" s="32"/>
-      <c r="AP15" s="16" t="s">
+      <c r="AL15" s="37"/>
+      <c r="AN15" s="45"/>
+      <c r="AO15" s="45"/>
+      <c r="AP15" s="37" t="s">
         <v>171</v>
       </c>
-      <c r="AQ15" s="16"/>
+      <c r="AQ15" s="37"/>
     </row>
     <row r="16" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="16" t="s">
+      <c r="C16" s="40"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="H16" s="16"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="16" t="s">
+      <c r="H16" s="37"/>
+      <c r="J16" s="45"/>
+      <c r="K16" s="45"/>
+      <c r="L16" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="M16" s="16"/>
-      <c r="O16" s="32"/>
-      <c r="P16" s="32"/>
-      <c r="Q16" s="16" t="s">
+      <c r="M16" s="37"/>
+      <c r="O16" s="45"/>
+      <c r="P16" s="45"/>
+      <c r="Q16" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="R16" s="16"/>
-      <c r="T16" s="32"/>
-      <c r="U16" s="32"/>
-      <c r="V16" s="16" t="s">
+      <c r="R16" s="37"/>
+      <c r="T16" s="45"/>
+      <c r="U16" s="45"/>
+      <c r="V16" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="W16" s="16"/>
-      <c r="Y16" s="32"/>
-      <c r="Z16" s="32"/>
-      <c r="AA16" s="16" t="s">
+      <c r="W16" s="37"/>
+      <c r="Y16" s="45"/>
+      <c r="Z16" s="45"/>
+      <c r="AA16" s="37" t="s">
         <v>121</v>
       </c>
-      <c r="AB16" s="16"/>
-      <c r="AD16" s="32"/>
-      <c r="AE16" s="32"/>
-      <c r="AF16" s="16" t="s">
+      <c r="AB16" s="37"/>
+      <c r="AD16" s="45"/>
+      <c r="AE16" s="45"/>
+      <c r="AF16" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="AG16" s="16"/>
-      <c r="AI16" s="32"/>
-      <c r="AJ16" s="32"/>
-      <c r="AK16" s="16" t="s">
+      <c r="AG16" s="37"/>
+      <c r="AI16" s="45"/>
+      <c r="AJ16" s="45"/>
+      <c r="AK16" s="37" t="s">
         <v>144</v>
       </c>
-      <c r="AL16" s="16"/>
-      <c r="AN16" s="32"/>
-      <c r="AO16" s="32"/>
-      <c r="AP16" s="16" t="s">
+      <c r="AL16" s="37"/>
+      <c r="AN16" s="45"/>
+      <c r="AO16" s="45"/>
+      <c r="AP16" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="AQ16" s="16"/>
+      <c r="AQ16" s="37"/>
     </row>
     <row r="17" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="C17" s="20"/>
+      <c r="C17" s="40"/>
       <c r="D17" s="11"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="16" t="s">
+      <c r="E17" s="48"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="H17" s="16"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="16" t="s">
+      <c r="H17" s="37"/>
+      <c r="J17" s="45"/>
+      <c r="K17" s="45"/>
+      <c r="L17" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="M17" s="16"/>
-      <c r="O17" s="32"/>
-      <c r="P17" s="32"/>
-      <c r="Q17" s="19" t="s">
+      <c r="M17" s="37"/>
+      <c r="O17" s="45"/>
+      <c r="P17" s="45"/>
+      <c r="Q17" s="39" t="s">
         <v>131</v>
       </c>
-      <c r="R17" s="20"/>
-      <c r="T17" s="32"/>
-      <c r="U17" s="32"/>
-      <c r="V17" s="16" t="s">
+      <c r="R17" s="40"/>
+      <c r="T17" s="45"/>
+      <c r="U17" s="45"/>
+      <c r="V17" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="W17" s="16"/>
-      <c r="Y17" s="32"/>
-      <c r="Z17" s="32"/>
-      <c r="AA17" s="16" t="s">
+      <c r="W17" s="37"/>
+      <c r="Y17" s="45"/>
+      <c r="Z17" s="45"/>
+      <c r="AA17" s="37" t="s">
         <v>122</v>
       </c>
-      <c r="AB17" s="16"/>
-      <c r="AD17" s="32"/>
-      <c r="AE17" s="32"/>
-      <c r="AF17" s="16" t="s">
+      <c r="AB17" s="37"/>
+      <c r="AD17" s="45"/>
+      <c r="AE17" s="45"/>
+      <c r="AF17" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="AG17" s="16"/>
-      <c r="AI17" s="32"/>
-      <c r="AJ17" s="32"/>
-      <c r="AK17" s="16" t="s">
+      <c r="AG17" s="37"/>
+      <c r="AI17" s="45"/>
+      <c r="AJ17" s="45"/>
+      <c r="AK17" s="37" t="s">
         <v>141</v>
       </c>
-      <c r="AL17" s="16"/>
-      <c r="AN17" s="32"/>
-      <c r="AO17" s="32"/>
-      <c r="AP17" s="16" t="s">
+      <c r="AL17" s="37"/>
+      <c r="AN17" s="45"/>
+      <c r="AO17" s="45"/>
+      <c r="AP17" s="37" t="s">
         <v>191</v>
       </c>
-      <c r="AQ17" s="16"/>
+      <c r="AQ17" s="37"/>
     </row>
     <row r="18" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="20"/>
+      <c r="C18" s="40"/>
       <c r="D18" s="8"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="16" t="s">
+      <c r="E18" s="48"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="H18" s="16"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="32"/>
-      <c r="L18" s="16" t="s">
+      <c r="H18" s="37"/>
+      <c r="J18" s="45"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="M18" s="16"/>
-      <c r="O18" s="32"/>
-      <c r="P18" s="32"/>
-      <c r="Q18" s="16" t="s">
+      <c r="M18" s="37"/>
+      <c r="O18" s="45"/>
+      <c r="P18" s="45"/>
+      <c r="Q18" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="R18" s="16"/>
-      <c r="T18" s="32"/>
-      <c r="U18" s="32"/>
-      <c r="V18" s="16" t="s">
+      <c r="R18" s="37"/>
+      <c r="T18" s="45"/>
+      <c r="U18" s="45"/>
+      <c r="V18" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="W18" s="16"/>
-      <c r="Y18" s="32"/>
-      <c r="Z18" s="32"/>
-      <c r="AA18" s="16" t="s">
+      <c r="W18" s="37"/>
+      <c r="Y18" s="45"/>
+      <c r="Z18" s="45"/>
+      <c r="AA18" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="AB18" s="16"/>
-      <c r="AD18" s="32"/>
-      <c r="AE18" s="32"/>
-      <c r="AF18" s="16" t="s">
+      <c r="AB18" s="37"/>
+      <c r="AD18" s="45"/>
+      <c r="AE18" s="45"/>
+      <c r="AF18" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="AG18" s="16"/>
-      <c r="AI18" s="32"/>
-      <c r="AJ18" s="32"/>
-      <c r="AK18" s="16" t="s">
+      <c r="AG18" s="37"/>
+      <c r="AI18" s="45"/>
+      <c r="AJ18" s="45"/>
+      <c r="AK18" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="AL18" s="16"/>
-      <c r="AN18" s="32"/>
-      <c r="AO18" s="32"/>
-      <c r="AP18" s="16" t="s">
+      <c r="AL18" s="37"/>
+      <c r="AN18" s="45"/>
+      <c r="AO18" s="45"/>
+      <c r="AP18" s="37" t="s">
         <v>190</v>
       </c>
-      <c r="AQ18" s="16"/>
+      <c r="AQ18" s="37"/>
     </row>
     <row r="19" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="20"/>
+      <c r="C19" s="40"/>
       <c r="D19" s="8"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="16" t="s">
+      <c r="E19" s="48"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="H19" s="16"/>
-      <c r="J19" s="32"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="16" t="s">
+      <c r="H19" s="37"/>
+      <c r="J19" s="45"/>
+      <c r="K19" s="45"/>
+      <c r="L19" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="M19" s="16"/>
-      <c r="O19" s="32"/>
-      <c r="P19" s="32"/>
-      <c r="Q19" s="16" t="s">
+      <c r="M19" s="37"/>
+      <c r="O19" s="45"/>
+      <c r="P19" s="45"/>
+      <c r="Q19" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="R19" s="16"/>
-      <c r="T19" s="32"/>
-      <c r="U19" s="32"/>
-      <c r="V19" s="16" t="s">
+      <c r="R19" s="37"/>
+      <c r="T19" s="45"/>
+      <c r="U19" s="45"/>
+      <c r="V19" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="W19" s="16"/>
-      <c r="Y19" s="32"/>
-      <c r="Z19" s="32"/>
-      <c r="AA19" s="16" t="s">
+      <c r="W19" s="37"/>
+      <c r="Y19" s="45"/>
+      <c r="Z19" s="45"/>
+      <c r="AA19" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="AB19" s="16"/>
-      <c r="AD19" s="32"/>
-      <c r="AE19" s="32"/>
-      <c r="AF19" s="16" t="s">
+      <c r="AB19" s="37"/>
+      <c r="AD19" s="45"/>
+      <c r="AE19" s="45"/>
+      <c r="AF19" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="AG19" s="16"/>
-      <c r="AI19" s="32"/>
-      <c r="AJ19" s="32"/>
-      <c r="AK19" s="16" t="s">
+      <c r="AG19" s="37"/>
+      <c r="AI19" s="45"/>
+      <c r="AJ19" s="45"/>
+      <c r="AK19" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="AL19" s="16"/>
-      <c r="AN19" s="32"/>
-      <c r="AO19" s="32"/>
-      <c r="AP19" s="16" t="s">
+      <c r="AL19" s="37"/>
+      <c r="AN19" s="45"/>
+      <c r="AO19" s="45"/>
+      <c r="AP19" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="AQ19" s="16"/>
+      <c r="AQ19" s="37"/>
     </row>
     <row r="20" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="C20" s="20"/>
+      <c r="C20" s="40"/>
       <c r="D20" s="8"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="16" t="s">
+      <c r="E20" s="48"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="H20" s="16"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="16" t="s">
+      <c r="H20" s="37"/>
+      <c r="J20" s="45"/>
+      <c r="K20" s="45"/>
+      <c r="L20" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="M20" s="16"/>
-      <c r="O20" s="32"/>
-      <c r="P20" s="32"/>
-      <c r="Q20" s="16" t="s">
+      <c r="M20" s="37"/>
+      <c r="O20" s="45"/>
+      <c r="P20" s="45"/>
+      <c r="Q20" s="37" t="s">
         <v>129</v>
       </c>
-      <c r="R20" s="16"/>
-      <c r="T20" s="32"/>
-      <c r="U20" s="32"/>
-      <c r="V20" s="16" t="s">
+      <c r="R20" s="37"/>
+      <c r="T20" s="45"/>
+      <c r="U20" s="45"/>
+      <c r="V20" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="W20" s="16"/>
-      <c r="Y20" s="32"/>
-      <c r="Z20" s="32"/>
-      <c r="AA20" s="16" t="s">
+      <c r="W20" s="37"/>
+      <c r="Y20" s="45"/>
+      <c r="Z20" s="45"/>
+      <c r="AA20" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="AB20" s="16"/>
-      <c r="AD20" s="32"/>
-      <c r="AE20" s="32"/>
-      <c r="AF20" s="16" t="s">
+      <c r="AB20" s="37"/>
+      <c r="AD20" s="45"/>
+      <c r="AE20" s="45"/>
+      <c r="AF20" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="AG20" s="16"/>
-      <c r="AI20" s="32"/>
-      <c r="AJ20" s="32"/>
-      <c r="AK20" s="16" t="s">
+      <c r="AG20" s="37"/>
+      <c r="AI20" s="45"/>
+      <c r="AJ20" s="45"/>
+      <c r="AK20" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="AL20" s="16"/>
-      <c r="AN20" s="32"/>
-      <c r="AO20" s="32"/>
-      <c r="AP20" s="16" t="s">
+      <c r="AL20" s="37"/>
+      <c r="AN20" s="45"/>
+      <c r="AO20" s="45"/>
+      <c r="AP20" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="AQ20" s="16"/>
+      <c r="AQ20" s="37"/>
     </row>
     <row r="21" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="20"/>
+      <c r="C21" s="40"/>
       <c r="D21" s="8"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="16" t="s">
+      <c r="E21" s="48"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="H21" s="16"/>
-      <c r="O21" s="32"/>
-      <c r="P21" s="32"/>
-      <c r="Q21" s="19" t="s">
+      <c r="H21" s="37"/>
+      <c r="O21" s="45"/>
+      <c r="P21" s="45"/>
+      <c r="Q21" s="39" t="s">
         <v>162</v>
       </c>
-      <c r="R21" s="20"/>
-      <c r="T21" s="32"/>
-      <c r="U21" s="32"/>
-      <c r="V21" s="16" t="s">
+      <c r="R21" s="40"/>
+      <c r="T21" s="45"/>
+      <c r="U21" s="45"/>
+      <c r="V21" s="37" t="s">
         <v>113</v>
       </c>
-      <c r="W21" s="16"/>
-      <c r="Y21" s="32"/>
-      <c r="Z21" s="32"/>
-      <c r="AA21" s="16" t="s">
+      <c r="W21" s="37"/>
+      <c r="Y21" s="45"/>
+      <c r="Z21" s="45"/>
+      <c r="AA21" s="37" t="s">
         <v>127</v>
       </c>
-      <c r="AB21" s="16"/>
-      <c r="AD21" s="32"/>
-      <c r="AE21" s="32"/>
-      <c r="AF21" s="16" t="s">
+      <c r="AB21" s="37"/>
+      <c r="AD21" s="45"/>
+      <c r="AE21" s="45"/>
+      <c r="AF21" s="37" t="s">
         <v>138</v>
       </c>
-      <c r="AG21" s="16"/>
-      <c r="AI21" s="32"/>
-      <c r="AJ21" s="32"/>
-      <c r="AK21" s="16" t="s">
+      <c r="AG21" s="37"/>
+      <c r="AI21" s="45"/>
+      <c r="AJ21" s="45"/>
+      <c r="AK21" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="AL21" s="16"/>
+      <c r="AL21" s="37"/>
     </row>
     <row r="22" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="C22" s="20"/>
+      <c r="C22" s="40"/>
       <c r="D22" s="8"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="16" t="s">
+      <c r="E22" s="48"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="H22" s="16"/>
-      <c r="J22" s="17" t="s">
+      <c r="H22" s="37"/>
+      <c r="J22" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="K22" s="17"/>
-      <c r="L22" s="22" t="s">
+      <c r="K22" s="43"/>
+      <c r="L22" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="M22" s="22"/>
-      <c r="O22" s="32"/>
-      <c r="P22" s="32"/>
-      <c r="Q22" s="19" t="s">
+      <c r="M22" s="44"/>
+      <c r="O22" s="45"/>
+      <c r="P22" s="45"/>
+      <c r="Q22" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="R22" s="20"/>
+      <c r="R22" s="40"/>
       <c r="S22" s="8"/>
-      <c r="T22" s="32"/>
-      <c r="U22" s="32"/>
-      <c r="V22" s="16" t="s">
+      <c r="T22" s="45"/>
+      <c r="U22" s="45"/>
+      <c r="V22" s="37" t="s">
         <v>114</v>
       </c>
-      <c r="W22" s="16"/>
-      <c r="Y22" s="32"/>
-      <c r="Z22" s="32"/>
-      <c r="AA22" s="16" t="s">
+      <c r="W22" s="37"/>
+      <c r="Y22" s="45"/>
+      <c r="Z22" s="45"/>
+      <c r="AA22" s="37" t="s">
         <v>128</v>
       </c>
-      <c r="AB22" s="16"/>
-      <c r="AD22" s="32"/>
-      <c r="AE22" s="32"/>
-      <c r="AF22" s="16" t="s">
+      <c r="AB22" s="37"/>
+      <c r="AD22" s="45"/>
+      <c r="AE22" s="45"/>
+      <c r="AF22" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="AG22" s="16"/>
+      <c r="AG22" s="37"/>
     </row>
     <row r="23" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="20"/>
+      <c r="C23" s="40"/>
       <c r="D23" s="8"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="16" t="s">
+      <c r="E23" s="48"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="H23" s="16"/>
-      <c r="J23" s="32" t="s">
+      <c r="H23" s="37"/>
+      <c r="J23" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="K23" s="32"/>
-      <c r="L23" s="16" t="s">
+      <c r="K23" s="45"/>
+      <c r="L23" s="37" t="s">
         <v>143</v>
       </c>
-      <c r="M23" s="16"/>
-      <c r="O23" s="32"/>
-      <c r="P23" s="32"/>
-      <c r="Q23" s="19" t="s">
+      <c r="M23" s="37"/>
+      <c r="O23" s="45"/>
+      <c r="P23" s="45"/>
+      <c r="Q23" s="39" t="s">
         <v>163</v>
       </c>
-      <c r="R23" s="20"/>
+      <c r="R23" s="40"/>
       <c r="S23" s="8"/>
-      <c r="T23" s="32"/>
-      <c r="U23" s="32"/>
-      <c r="V23" s="16" t="s">
+      <c r="T23" s="45"/>
+      <c r="U23" s="45"/>
+      <c r="V23" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="W23" s="16"/>
-      <c r="Y23" s="32"/>
-      <c r="Z23" s="32"/>
-      <c r="AA23" s="16" t="s">
+      <c r="W23" s="37"/>
+      <c r="Y23" s="45"/>
+      <c r="Z23" s="45"/>
+      <c r="AA23" s="37" t="s">
         <v>199</v>
       </c>
-      <c r="AB23" s="16"/>
-      <c r="AD23" s="32"/>
-      <c r="AE23" s="32"/>
-      <c r="AF23" s="16" t="s">
+      <c r="AB23" s="37"/>
+      <c r="AD23" s="45"/>
+      <c r="AE23" s="45"/>
+      <c r="AF23" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="AG23" s="16"/>
+      <c r="AG23" s="37"/>
     </row>
     <row r="24" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="39" t="s">
         <v>157</v>
       </c>
-      <c r="C24" s="20"/>
+      <c r="C24" s="40"/>
       <c r="D24" s="8"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="16" t="s">
+      <c r="E24" s="48"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="H24" s="16"/>
-      <c r="J24" s="32"/>
-      <c r="K24" s="32"/>
-      <c r="L24" s="16" t="s">
+      <c r="H24" s="37"/>
+      <c r="J24" s="45"/>
+      <c r="K24" s="45"/>
+      <c r="L24" s="37" t="s">
         <v>144</v>
       </c>
-      <c r="M24" s="16"/>
-      <c r="O24" s="32"/>
-      <c r="P24" s="32"/>
-      <c r="Q24" s="16" t="s">
+      <c r="M24" s="37"/>
+      <c r="O24" s="45"/>
+      <c r="P24" s="45"/>
+      <c r="Q24" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="R24" s="16"/>
+      <c r="R24" s="37"/>
       <c r="S24" s="8"/>
-      <c r="T24" s="32"/>
-      <c r="U24" s="32"/>
-      <c r="V24" s="16" t="s">
+      <c r="T24" s="45"/>
+      <c r="U24" s="45"/>
+      <c r="V24" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="W24" s="16"/>
+      <c r="W24" s="37"/>
     </row>
     <row r="25" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="39" t="s">
         <v>158</v>
       </c>
-      <c r="C25" s="20"/>
+      <c r="C25" s="40"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="40"/>
-      <c r="G25" s="16" t="s">
+      <c r="E25" s="48"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="H25" s="16"/>
-      <c r="J25" s="32"/>
-      <c r="K25" s="32"/>
-      <c r="L25" s="16" t="s">
+      <c r="H25" s="37"/>
+      <c r="J25" s="45"/>
+      <c r="K25" s="45"/>
+      <c r="L25" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="M25" s="16"/>
-      <c r="Q25" s="15"/>
-      <c r="R25" s="15"/>
+      <c r="M25" s="37"/>
+      <c r="Q25" s="53"/>
+      <c r="R25" s="53"/>
       <c r="S25" s="8"/>
-      <c r="T25" s="32"/>
-      <c r="U25" s="32"/>
-      <c r="V25" s="16" t="s">
+      <c r="T25" s="45"/>
+      <c r="U25" s="45"/>
+      <c r="V25" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="W25" s="16"/>
+      <c r="W25" s="37"/>
     </row>
     <row r="26" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="20"/>
+      <c r="C26" s="40"/>
       <c r="D26" s="8"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="40"/>
-      <c r="G26" s="16" t="s">
+      <c r="E26" s="48"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="H26" s="16"/>
-      <c r="J26" s="32"/>
-      <c r="K26" s="32"/>
-      <c r="L26" s="16" t="s">
+      <c r="H26" s="37"/>
+      <c r="J26" s="45"/>
+      <c r="K26" s="45"/>
+      <c r="L26" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="M26" s="16"/>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="15"/>
+      <c r="M26" s="37"/>
+      <c r="Q26" s="53"/>
+      <c r="R26" s="53"/>
       <c r="S26" s="8"/>
       <c r="T26" s="8"/>
     </row>
     <row r="27" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="20"/>
+      <c r="C27" s="40"/>
       <c r="D27" s="8"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="40"/>
-      <c r="G27" s="19" t="s">
+      <c r="E27" s="48"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="H27" s="20"/>
-      <c r="Q27" s="15"/>
-      <c r="R27" s="15"/>
+      <c r="H27" s="40"/>
+      <c r="Q27" s="53"/>
+      <c r="R27" s="53"/>
       <c r="S27" s="8"/>
       <c r="T27" s="8"/>
     </row>
     <row r="28" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="C28" s="16"/>
+      <c r="C28" s="37"/>
       <c r="D28" s="8"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="40"/>
-      <c r="G28" s="16" t="s">
+      <c r="E28" s="48"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="H28" s="16"/>
-      <c r="J28" s="17" t="s">
+      <c r="H28" s="37"/>
+      <c r="J28" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="K28" s="17"/>
-      <c r="L28" s="22" t="s">
+      <c r="K28" s="43"/>
+      <c r="L28" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="M28" s="22"/>
-      <c r="O28" s="17" t="s">
+      <c r="M28" s="44"/>
+      <c r="O28" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="P28" s="17"/>
-      <c r="Q28" s="22" t="s">
+      <c r="P28" s="43"/>
+      <c r="Q28" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="R28" s="22"/>
-      <c r="T28" s="17" t="s">
+      <c r="R28" s="44"/>
+      <c r="T28" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="U28" s="17"/>
-      <c r="V28" s="22" t="s">
+      <c r="U28" s="43"/>
+      <c r="V28" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="W28" s="22"/>
-      <c r="Y28" s="17" t="s">
+      <c r="W28" s="44"/>
+      <c r="Y28" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="Z28" s="17"/>
-      <c r="AA28" s="22" t="s">
+      <c r="Z28" s="43"/>
+      <c r="AA28" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="AB28" s="22"/>
-      <c r="AD28" s="17" t="s">
+      <c r="AB28" s="44"/>
+      <c r="AD28" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="AE28" s="17"/>
-      <c r="AF28" s="22" t="s">
+      <c r="AE28" s="43"/>
+      <c r="AF28" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="AG28" s="22"/>
-      <c r="AI28" s="17" t="s">
+      <c r="AG28" s="44"/>
+      <c r="AI28" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="AJ28" s="17"/>
-      <c r="AK28" s="22" t="s">
+      <c r="AJ28" s="43"/>
+      <c r="AK28" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="AL28" s="22"/>
-      <c r="AN28" s="17" t="s">
+      <c r="AL28" s="44"/>
+      <c r="AN28" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="AO28" s="17"/>
-      <c r="AP28" s="22" t="s">
+      <c r="AO28" s="43"/>
+      <c r="AP28" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="AQ28" s="22"/>
+      <c r="AQ28" s="44"/>
     </row>
     <row r="29" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="37" t="s">
         <v>185</v>
       </c>
-      <c r="C29" s="16"/>
+      <c r="C29" s="37"/>
       <c r="D29" s="8"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="16" t="s">
+      <c r="E29" s="48"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="H29" s="16"/>
-      <c r="J29" s="32" t="s">
+      <c r="H29" s="37"/>
+      <c r="J29" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="K29" s="32"/>
-      <c r="L29" s="16" t="s">
+      <c r="K29" s="45"/>
+      <c r="L29" s="37" t="s">
         <v>145</v>
       </c>
-      <c r="M29" s="16"/>
-      <c r="O29" s="32" t="s">
+      <c r="M29" s="37"/>
+      <c r="O29" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="P29" s="32"/>
-      <c r="Q29" s="16" t="s">
+      <c r="P29" s="45"/>
+      <c r="Q29" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="R29" s="16"/>
-      <c r="T29" s="32" t="s">
+      <c r="R29" s="37"/>
+      <c r="T29" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="U29" s="32"/>
-      <c r="V29" s="16" t="s">
+      <c r="U29" s="45"/>
+      <c r="V29" s="37" t="s">
         <v>153</v>
       </c>
-      <c r="W29" s="16"/>
-      <c r="Y29" s="32" t="s">
+      <c r="W29" s="37"/>
+      <c r="Y29" s="45" t="s">
         <v>157</v>
       </c>
-      <c r="Z29" s="32"/>
-      <c r="AA29" s="16" t="s">
+      <c r="Z29" s="45"/>
+      <c r="AA29" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="AB29" s="16"/>
-      <c r="AD29" s="32" t="s">
+      <c r="AB29" s="37"/>
+      <c r="AD29" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="AE29" s="32"/>
-      <c r="AF29" s="16" t="s">
+      <c r="AE29" s="45"/>
+      <c r="AF29" s="37" t="s">
         <v>174</v>
       </c>
-      <c r="AG29" s="16"/>
-      <c r="AI29" s="32" t="s">
+      <c r="AG29" s="37"/>
+      <c r="AI29" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="AJ29" s="32"/>
-      <c r="AK29" s="16" t="s">
+      <c r="AJ29" s="45"/>
+      <c r="AK29" s="37" t="s">
         <v>178</v>
       </c>
-      <c r="AL29" s="16"/>
-      <c r="AN29" s="32" t="s">
+      <c r="AL29" s="37"/>
+      <c r="AN29" s="45" t="s">
         <v>192</v>
       </c>
-      <c r="AO29" s="32"/>
-      <c r="AP29" s="16" t="s">
+      <c r="AO29" s="45"/>
+      <c r="AP29" s="37" t="s">
         <v>193</v>
       </c>
-      <c r="AQ29" s="16"/>
+      <c r="AQ29" s="37"/>
     </row>
     <row r="30" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="37" t="s">
         <v>187</v>
       </c>
-      <c r="C30" s="16"/>
+      <c r="C30" s="37"/>
       <c r="D30" s="8"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="19" t="s">
+      <c r="E30" s="48"/>
+      <c r="F30" s="49"/>
+      <c r="G30" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="H30" s="20"/>
-      <c r="J30" s="32"/>
-      <c r="K30" s="32"/>
-      <c r="L30" s="16" t="s">
+      <c r="H30" s="40"/>
+      <c r="J30" s="45"/>
+      <c r="K30" s="45"/>
+      <c r="L30" s="37" t="s">
         <v>114</v>
       </c>
-      <c r="M30" s="16"/>
-      <c r="O30" s="32"/>
-      <c r="P30" s="32"/>
-      <c r="Q30" s="16" t="s">
+      <c r="M30" s="37"/>
+      <c r="O30" s="45"/>
+      <c r="P30" s="45"/>
+      <c r="Q30" s="37" t="s">
         <v>149</v>
       </c>
-      <c r="R30" s="16"/>
-      <c r="T30" s="32"/>
-      <c r="U30" s="32"/>
-      <c r="V30" s="16" t="s">
+      <c r="R30" s="37"/>
+      <c r="T30" s="45"/>
+      <c r="U30" s="45"/>
+      <c r="V30" s="37" t="s">
         <v>154</v>
       </c>
-      <c r="W30" s="16"/>
-      <c r="Y30" s="32"/>
-      <c r="Z30" s="32"/>
-      <c r="AA30" s="16" t="s">
+      <c r="W30" s="37"/>
+      <c r="Y30" s="45"/>
+      <c r="Z30" s="45"/>
+      <c r="AA30" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="AB30" s="16"/>
-      <c r="AD30" s="32"/>
-      <c r="AE30" s="32"/>
-      <c r="AF30" s="16" t="s">
+      <c r="AB30" s="37"/>
+      <c r="AD30" s="45"/>
+      <c r="AE30" s="45"/>
+      <c r="AF30" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="AG30" s="16"/>
-      <c r="AI30" s="32"/>
-      <c r="AJ30" s="32"/>
-      <c r="AK30" s="16" t="s">
+      <c r="AG30" s="37"/>
+      <c r="AI30" s="45"/>
+      <c r="AJ30" s="45"/>
+      <c r="AK30" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="AL30" s="16"/>
-      <c r="AN30" s="32"/>
-      <c r="AO30" s="32"/>
-      <c r="AP30" s="16" t="s">
+      <c r="AL30" s="37"/>
+      <c r="AN30" s="45"/>
+      <c r="AO30" s="45"/>
+      <c r="AP30" s="37" t="s">
         <v>194</v>
       </c>
-      <c r="AQ30" s="16"/>
+      <c r="AQ30" s="37"/>
     </row>
     <row r="31" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="37" t="s">
         <v>192</v>
       </c>
-      <c r="C31" s="16"/>
+      <c r="C31" s="37"/>
       <c r="D31" s="8"/>
-      <c r="E31" s="41"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="16" t="s">
+      <c r="E31" s="50"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="H31" s="16"/>
-      <c r="J31" s="32"/>
-      <c r="K31" s="32"/>
-      <c r="L31" s="16" t="s">
+      <c r="H31" s="37"/>
+      <c r="J31" s="45"/>
+      <c r="K31" s="45"/>
+      <c r="L31" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="M31" s="16"/>
-      <c r="O31" s="32"/>
-      <c r="P31" s="32"/>
-      <c r="Q31" s="16" t="s">
+      <c r="M31" s="37"/>
+      <c r="O31" s="45"/>
+      <c r="P31" s="45"/>
+      <c r="Q31" s="37" t="s">
         <v>150</v>
       </c>
-      <c r="R31" s="16"/>
-      <c r="T31" s="32"/>
-      <c r="U31" s="32"/>
-      <c r="V31" s="16" t="s">
+      <c r="R31" s="37"/>
+      <c r="T31" s="45"/>
+      <c r="U31" s="45"/>
+      <c r="V31" s="37" t="s">
         <v>155</v>
       </c>
-      <c r="W31" s="16"/>
-      <c r="Y31" s="32"/>
-      <c r="Z31" s="32"/>
-      <c r="AA31" s="16" t="s">
+      <c r="W31" s="37"/>
+      <c r="Y31" s="45"/>
+      <c r="Z31" s="45"/>
+      <c r="AA31" s="37" t="s">
         <v>159</v>
       </c>
-      <c r="AB31" s="16"/>
-      <c r="AD31" s="32"/>
-      <c r="AE31" s="32"/>
-      <c r="AF31" s="16" t="s">
+      <c r="AB31" s="37"/>
+      <c r="AD31" s="45"/>
+      <c r="AE31" s="45"/>
+      <c r="AF31" s="37" t="s">
         <v>171</v>
       </c>
-      <c r="AG31" s="16"/>
-      <c r="AI31" s="32"/>
-      <c r="AJ31" s="32"/>
-      <c r="AK31" s="16" t="s">
+      <c r="AG31" s="37"/>
+      <c r="AI31" s="45"/>
+      <c r="AJ31" s="45"/>
+      <c r="AK31" s="37" t="s">
         <v>179</v>
       </c>
-      <c r="AL31" s="16"/>
-      <c r="AN31" s="32"/>
-      <c r="AO31" s="32"/>
-      <c r="AP31" s="16" t="s">
+      <c r="AL31" s="37"/>
+      <c r="AN31" s="45"/>
+      <c r="AO31" s="45"/>
+      <c r="AP31" s="37" t="s">
         <v>195</v>
       </c>
-      <c r="AQ31" s="16"/>
+      <c r="AQ31" s="37"/>
     </row>
     <row r="32" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="C32" s="16"/>
+      <c r="C32" s="37"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
-      <c r="J32" s="32"/>
-      <c r="K32" s="32"/>
-      <c r="L32" s="16" t="s">
+      <c r="J32" s="45"/>
+      <c r="K32" s="45"/>
+      <c r="L32" s="37" t="s">
         <v>147</v>
       </c>
-      <c r="M32" s="16"/>
-      <c r="O32" s="32"/>
-      <c r="P32" s="32"/>
-      <c r="Q32" s="16" t="s">
+      <c r="M32" s="37"/>
+      <c r="O32" s="45"/>
+      <c r="P32" s="45"/>
+      <c r="Q32" s="37" t="s">
         <v>151</v>
       </c>
-      <c r="R32" s="16"/>
-      <c r="T32" s="32"/>
-      <c r="U32" s="32"/>
-      <c r="V32" s="16" t="s">
+      <c r="R32" s="37"/>
+      <c r="T32" s="45"/>
+      <c r="U32" s="45"/>
+      <c r="V32" s="37" t="s">
         <v>156</v>
       </c>
-      <c r="W32" s="16"/>
-      <c r="Y32" s="32"/>
-      <c r="Z32" s="32"/>
-      <c r="AA32" s="16" t="s">
+      <c r="W32" s="37"/>
+      <c r="Y32" s="45"/>
+      <c r="Z32" s="45"/>
+      <c r="AA32" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="AB32" s="16"/>
-      <c r="AD32" s="32"/>
-      <c r="AE32" s="32"/>
-      <c r="AF32" s="16" t="s">
+      <c r="AB32" s="37"/>
+      <c r="AD32" s="45"/>
+      <c r="AE32" s="45"/>
+      <c r="AF32" s="37" t="s">
         <v>173</v>
       </c>
-      <c r="AG32" s="16"/>
-      <c r="AI32" s="32"/>
-      <c r="AJ32" s="32"/>
-      <c r="AK32" s="16" t="s">
+      <c r="AG32" s="37"/>
+      <c r="AI32" s="45"/>
+      <c r="AJ32" s="45"/>
+      <c r="AK32" s="37" t="s">
         <v>181</v>
       </c>
-      <c r="AL32" s="16"/>
-      <c r="AN32" s="32"/>
-      <c r="AO32" s="32"/>
-      <c r="AP32" s="16" t="s">
+      <c r="AL32" s="37"/>
+      <c r="AN32" s="45"/>
+      <c r="AO32" s="45"/>
+      <c r="AP32" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="AQ32" s="16"/>
+      <c r="AQ32" s="37"/>
     </row>
     <row r="33" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B33" s="16" t="s">
+      <c r="B33" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="C33" s="16"/>
+      <c r="C33" s="37"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
-      <c r="J33" s="32"/>
-      <c r="K33" s="32"/>
-      <c r="L33" s="16" t="s">
+      <c r="J33" s="45"/>
+      <c r="K33" s="45"/>
+      <c r="L33" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="M33" s="16"/>
-      <c r="O33" s="32"/>
-      <c r="P33" s="32"/>
-      <c r="Q33" s="16" t="s">
+      <c r="M33" s="37"/>
+      <c r="O33" s="45"/>
+      <c r="P33" s="45"/>
+      <c r="Q33" s="37" t="s">
         <v>143</v>
       </c>
-      <c r="R33" s="16"/>
-      <c r="T33" s="32"/>
-      <c r="U33" s="32"/>
-      <c r="V33" s="33" t="s">
+      <c r="R33" s="37"/>
+      <c r="T33" s="45"/>
+      <c r="U33" s="45"/>
+      <c r="V33" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="W33" s="33"/>
-      <c r="Y33" s="32"/>
-      <c r="Z33" s="32"/>
-      <c r="AA33" s="16" t="s">
+      <c r="W33" s="54"/>
+      <c r="Y33" s="45"/>
+      <c r="Z33" s="45"/>
+      <c r="AA33" s="37" t="s">
         <v>160</v>
       </c>
-      <c r="AB33" s="16"/>
-      <c r="AD33" s="32"/>
-      <c r="AE33" s="32"/>
-      <c r="AF33" s="16" t="s">
+      <c r="AB33" s="37"/>
+      <c r="AD33" s="45"/>
+      <c r="AE33" s="45"/>
+      <c r="AF33" s="37" t="s">
         <v>175</v>
       </c>
-      <c r="AG33" s="16"/>
-      <c r="AI33" s="32"/>
-      <c r="AJ33" s="32"/>
-      <c r="AK33" s="16" t="s">
+      <c r="AG33" s="37"/>
+      <c r="AI33" s="45"/>
+      <c r="AJ33" s="45"/>
+      <c r="AK33" s="37" t="s">
         <v>180</v>
       </c>
-      <c r="AL33" s="16"/>
-      <c r="AN33" s="32" t="s">
+      <c r="AL33" s="37"/>
+      <c r="AN33" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="AO33" s="32"/>
-      <c r="AP33" s="16" t="s">
+      <c r="AO33" s="45"/>
+      <c r="AP33" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="AQ33" s="16"/>
+      <c r="AQ33" s="37"/>
     </row>
     <row r="34" spans="2:43" x14ac:dyDescent="0.3">
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
-      <c r="J34" s="32"/>
-      <c r="K34" s="32"/>
-      <c r="L34" s="16" t="s">
+      <c r="J34" s="45"/>
+      <c r="K34" s="45"/>
+      <c r="L34" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="M34" s="16"/>
-      <c r="O34" s="32"/>
-      <c r="P34" s="32"/>
-      <c r="Q34" s="16" t="s">
+      <c r="M34" s="37"/>
+      <c r="O34" s="45"/>
+      <c r="P34" s="45"/>
+      <c r="Q34" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="R34" s="16"/>
-      <c r="Y34" s="32"/>
-      <c r="Z34" s="32"/>
-      <c r="AA34" s="16" t="s">
+      <c r="R34" s="37"/>
+      <c r="Y34" s="45"/>
+      <c r="Z34" s="45"/>
+      <c r="AA34" s="37" t="s">
         <v>161</v>
       </c>
-      <c r="AB34" s="16"/>
-      <c r="AD34" s="32"/>
-      <c r="AE34" s="32"/>
-      <c r="AF34" s="16" t="s">
+      <c r="AB34" s="37"/>
+      <c r="AD34" s="45"/>
+      <c r="AE34" s="45"/>
+      <c r="AF34" s="37" t="s">
         <v>176</v>
       </c>
-      <c r="AG34" s="16"/>
-      <c r="AI34" s="32"/>
-      <c r="AJ34" s="32"/>
-      <c r="AK34" s="16" t="s">
+      <c r="AG34" s="37"/>
+      <c r="AI34" s="45"/>
+      <c r="AJ34" s="45"/>
+      <c r="AK34" s="37" t="s">
         <v>183</v>
       </c>
-      <c r="AL34" s="16"/>
-      <c r="AN34" s="32"/>
-      <c r="AO34" s="32"/>
-      <c r="AP34" s="16" t="s">
+      <c r="AL34" s="37"/>
+      <c r="AN34" s="45"/>
+      <c r="AO34" s="45"/>
+      <c r="AP34" s="37" t="s">
         <v>196</v>
       </c>
-      <c r="AQ34" s="16"/>
+      <c r="AQ34" s="37"/>
     </row>
     <row r="35" spans="2:43" x14ac:dyDescent="0.3">
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
-      <c r="J35" s="32"/>
-      <c r="K35" s="32"/>
-      <c r="L35" s="16" t="s">
+      <c r="J35" s="45"/>
+      <c r="K35" s="45"/>
+      <c r="L35" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="M35" s="16"/>
-      <c r="O35" s="32"/>
-      <c r="P35" s="32"/>
-      <c r="Q35" s="16" t="s">
+      <c r="M35" s="37"/>
+      <c r="O35" s="45"/>
+      <c r="P35" s="45"/>
+      <c r="Q35" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="R35" s="16"/>
-      <c r="T35" s="17" t="s">
+      <c r="R35" s="37"/>
+      <c r="T35" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="U35" s="17"/>
-      <c r="V35" s="22" t="s">
+      <c r="U35" s="43"/>
+      <c r="V35" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="W35" s="22"/>
-      <c r="Y35" s="32"/>
-      <c r="Z35" s="32"/>
-      <c r="AA35" s="16" t="s">
+      <c r="W35" s="44"/>
+      <c r="Y35" s="45"/>
+      <c r="Z35" s="45"/>
+      <c r="AA35" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="AB35" s="16"/>
-      <c r="AD35" s="32"/>
-      <c r="AE35" s="32"/>
-      <c r="AF35" s="16" t="s">
+      <c r="AB35" s="37"/>
+      <c r="AD35" s="45"/>
+      <c r="AE35" s="45"/>
+      <c r="AF35" s="37" t="s">
         <v>177</v>
       </c>
-      <c r="AG35" s="16"/>
-      <c r="AI35" s="32"/>
-      <c r="AJ35" s="32"/>
-      <c r="AK35" s="16" t="s">
+      <c r="AG35" s="37"/>
+      <c r="AI35" s="45"/>
+      <c r="AJ35" s="45"/>
+      <c r="AK35" s="37" t="s">
         <v>182</v>
       </c>
-      <c r="AL35" s="16"/>
-      <c r="AN35" s="32"/>
-      <c r="AO35" s="32"/>
-      <c r="AP35" s="16" t="s">
+      <c r="AL35" s="37"/>
+      <c r="AN35" s="45"/>
+      <c r="AO35" s="45"/>
+      <c r="AP35" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="AQ35" s="16"/>
+      <c r="AQ35" s="37"/>
     </row>
     <row r="36" spans="2:43" x14ac:dyDescent="0.3">
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
-      <c r="O36" s="32"/>
-      <c r="P36" s="32"/>
-      <c r="Q36" s="16" t="s">
+      <c r="O36" s="45"/>
+      <c r="P36" s="45"/>
+      <c r="Q36" s="37" t="s">
         <v>152</v>
       </c>
-      <c r="R36" s="16"/>
-      <c r="T36" s="16" t="s">
+      <c r="R36" s="37"/>
+      <c r="T36" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="U36" s="16"/>
-      <c r="V36" s="16" t="s">
+      <c r="U36" s="37"/>
+      <c r="V36" s="37" t="s">
         <v>198</v>
       </c>
-      <c r="W36" s="16"/>
-      <c r="Y36" s="32"/>
-      <c r="Z36" s="32"/>
-      <c r="AA36" s="16" t="s">
+      <c r="W36" s="37"/>
+      <c r="Y36" s="45"/>
+      <c r="Z36" s="45"/>
+      <c r="AA36" s="37" t="s">
         <v>163</v>
       </c>
-      <c r="AB36" s="16"/>
-      <c r="AD36" s="32"/>
-      <c r="AE36" s="32"/>
-      <c r="AF36" s="16" t="s">
+      <c r="AB36" s="37"/>
+      <c r="AD36" s="45"/>
+      <c r="AE36" s="45"/>
+      <c r="AF36" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="AG36" s="16"/>
-      <c r="AI36" s="32"/>
-      <c r="AJ36" s="32"/>
-      <c r="AK36" s="16" t="s">
+      <c r="AG36" s="37"/>
+      <c r="AI36" s="45"/>
+      <c r="AJ36" s="45"/>
+      <c r="AK36" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="AL36" s="16"/>
-      <c r="AN36" s="32"/>
-      <c r="AO36" s="32"/>
-      <c r="AP36" s="16" t="s">
+      <c r="AL36" s="37"/>
+      <c r="AN36" s="45"/>
+      <c r="AO36" s="45"/>
+      <c r="AP36" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="AQ36" s="16"/>
+      <c r="AQ36" s="37"/>
     </row>
     <row r="37" spans="2:43" x14ac:dyDescent="0.3">
       <c r="D37" s="8"/>
-      <c r="E37" s="17" t="s">
+      <c r="E37" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="F37" s="17"/>
-      <c r="G37" s="22" t="s">
+      <c r="F37" s="43"/>
+      <c r="G37" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="H37" s="22"/>
-      <c r="J37" s="17" t="s">
+      <c r="H37" s="44"/>
+      <c r="J37" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="K37" s="17"/>
-      <c r="L37" s="22" t="s">
+      <c r="K37" s="43"/>
+      <c r="L37" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="M37" s="22"/>
-      <c r="O37" s="32"/>
-      <c r="P37" s="32"/>
-      <c r="Q37" s="16" t="s">
+      <c r="M37" s="44"/>
+      <c r="O37" s="45"/>
+      <c r="P37" s="45"/>
+      <c r="Q37" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="R37" s="16"/>
+      <c r="R37" s="37"/>
       <c r="S37" s="8"/>
       <c r="T37" s="8"/>
-      <c r="Y37" s="32"/>
-      <c r="Z37" s="32"/>
-      <c r="AA37" s="16" t="s">
+      <c r="Y37" s="45"/>
+      <c r="Z37" s="45"/>
+      <c r="AA37" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="AB37" s="16"/>
-      <c r="AN37" s="32"/>
-      <c r="AO37" s="32"/>
-      <c r="AP37" s="16" t="s">
+      <c r="AB37" s="37"/>
+      <c r="AN37" s="45"/>
+      <c r="AO37" s="45"/>
+      <c r="AP37" s="37" t="s">
         <v>197</v>
       </c>
-      <c r="AQ37" s="16"/>
+      <c r="AQ37" s="37"/>
     </row>
     <row r="38" spans="2:43" x14ac:dyDescent="0.3">
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
-      <c r="E38" s="33" t="s">
+      <c r="E38" s="54" t="s">
         <v>185</v>
       </c>
-      <c r="F38" s="33"/>
-      <c r="G38" s="16" t="s">
+      <c r="F38" s="54"/>
+      <c r="G38" s="37" t="s">
         <v>184</v>
       </c>
-      <c r="H38" s="16"/>
-      <c r="J38" s="32" t="s">
+      <c r="H38" s="37"/>
+      <c r="J38" s="45" t="s">
         <v>158</v>
       </c>
-      <c r="K38" s="32"/>
-      <c r="L38" s="16" t="s">
+      <c r="K38" s="45"/>
+      <c r="L38" s="37" t="s">
         <v>168</v>
       </c>
-      <c r="M38" s="16"/>
+      <c r="M38" s="37"/>
       <c r="Q38" s="8"/>
       <c r="R38" s="8"/>
       <c r="S38" s="8"/>
       <c r="T38" s="8"/>
-      <c r="Y38" s="32"/>
-      <c r="Z38" s="32"/>
-      <c r="AA38" s="16" t="s">
+      <c r="Y38" s="45"/>
+      <c r="Z38" s="45"/>
+      <c r="AA38" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="AB38" s="16"/>
-      <c r="AN38" s="32"/>
-      <c r="AO38" s="32"/>
-      <c r="AP38" s="16" t="s">
+      <c r="AB38" s="37"/>
+      <c r="AN38" s="45"/>
+      <c r="AO38" s="45"/>
+      <c r="AP38" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="AQ38" s="16"/>
+      <c r="AQ38" s="37"/>
     </row>
     <row r="39" spans="2:43" x14ac:dyDescent="0.3">
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
-      <c r="E39" s="33"/>
-      <c r="F39" s="33"/>
-      <c r="G39" s="16" t="s">
+      <c r="E39" s="54"/>
+      <c r="F39" s="54"/>
+      <c r="G39" s="37" t="s">
         <v>186</v>
       </c>
-      <c r="H39" s="16"/>
-      <c r="J39" s="32"/>
-      <c r="K39" s="32"/>
-      <c r="L39" s="16" t="s">
+      <c r="H39" s="37"/>
+      <c r="J39" s="45"/>
+      <c r="K39" s="45"/>
+      <c r="L39" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="M39" s="16"/>
+      <c r="M39" s="37"/>
       <c r="Q39" s="8"/>
       <c r="R39" s="8"/>
       <c r="S39" s="8"/>
       <c r="T39" s="8"/>
-      <c r="Y39" s="32"/>
-      <c r="Z39" s="32"/>
-      <c r="AA39" s="16" t="s">
+      <c r="Y39" s="45"/>
+      <c r="Z39" s="45"/>
+      <c r="AA39" s="37" t="s">
         <v>165</v>
       </c>
-      <c r="AB39" s="16"/>
+      <c r="AB39" s="37"/>
     </row>
     <row r="40" spans="2:43" x14ac:dyDescent="0.3">
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
       <c r="D40" s="8"/>
-      <c r="E40" s="33"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="16" t="s">
+      <c r="E40" s="54"/>
+      <c r="F40" s="54"/>
+      <c r="G40" s="37" t="s">
         <v>183</v>
       </c>
-      <c r="H40" s="16"/>
-      <c r="J40" s="32"/>
-      <c r="K40" s="32"/>
-      <c r="L40" s="16" t="s">
+      <c r="H40" s="37"/>
+      <c r="J40" s="45"/>
+      <c r="K40" s="45"/>
+      <c r="L40" s="37" t="s">
         <v>169</v>
       </c>
-      <c r="M40" s="16"/>
+      <c r="M40" s="37"/>
       <c r="Q40" s="8"/>
       <c r="R40" s="8"/>
       <c r="S40" s="8"/>
       <c r="T40" s="8"/>
-      <c r="Y40" s="32"/>
-      <c r="Z40" s="32"/>
-      <c r="AA40" s="16" t="s">
+      <c r="Y40" s="45"/>
+      <c r="Z40" s="45"/>
+      <c r="AA40" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="AB40" s="16"/>
+      <c r="AB40" s="37"/>
     </row>
     <row r="41" spans="2:43" x14ac:dyDescent="0.3">
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
-      <c r="E41" s="33"/>
-      <c r="F41" s="33"/>
-      <c r="G41" s="16" t="s">
+      <c r="E41" s="54"/>
+      <c r="F41" s="54"/>
+      <c r="G41" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="H41" s="16"/>
-      <c r="J41" s="32"/>
-      <c r="K41" s="32"/>
-      <c r="L41" s="16" t="s">
+      <c r="H41" s="37"/>
+      <c r="J41" s="45"/>
+      <c r="K41" s="45"/>
+      <c r="L41" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="M41" s="16"/>
+      <c r="M41" s="37"/>
       <c r="Q41" s="8"/>
       <c r="R41" s="8"/>
       <c r="S41" s="8"/>
       <c r="T41" s="8"/>
-      <c r="Y41" s="32"/>
-      <c r="Z41" s="32"/>
-      <c r="AA41" s="16" t="s">
+      <c r="Y41" s="45"/>
+      <c r="Z41" s="45"/>
+      <c r="AA41" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="AB41" s="16"/>
+      <c r="AB41" s="37"/>
     </row>
     <row r="42" spans="2:43" x14ac:dyDescent="0.3">
       <c r="B42" s="8"/>
@@ -3606,12 +3622,12 @@
       <c r="R42" s="8"/>
       <c r="S42" s="8"/>
       <c r="T42" s="8"/>
-      <c r="Y42" s="32"/>
-      <c r="Z42" s="32"/>
-      <c r="AA42" s="16" t="s">
+      <c r="Y42" s="45"/>
+      <c r="Z42" s="45"/>
+      <c r="AA42" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="AB42" s="16"/>
+      <c r="AB42" s="37"/>
     </row>
     <row r="43" spans="2:43" x14ac:dyDescent="0.3">
       <c r="B43" s="8"/>
@@ -3624,10 +3640,10 @@
       <c r="T43" s="8"/>
     </row>
     <row r="44" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B44" s="18" t="s">
+      <c r="B44" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="C44" s="18"/>
+      <c r="C44" s="64"/>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
       <c r="Q44" s="8"/>
@@ -3636,10 +3652,10 @@
       <c r="T44" s="8"/>
     </row>
     <row r="45" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B45" s="16" t="s">
+      <c r="B45" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="C45" s="16"/>
+      <c r="C45" s="37"/>
       <c r="D45" s="9"/>
       <c r="E45" s="9"/>
       <c r="Q45" s="9"/>
@@ -3648,10 +3664,10 @@
       <c r="T45" s="9"/>
     </row>
     <row r="46" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B46" s="16" t="s">
+      <c r="B46" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="C46" s="16"/>
+      <c r="C46" s="37"/>
       <c r="D46" s="9"/>
       <c r="E46" s="9"/>
       <c r="Q46" s="9"/>
@@ -3660,10 +3676,10 @@
       <c r="T46" s="9"/>
     </row>
     <row r="47" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="C47" s="16"/>
+      <c r="C47" s="37"/>
       <c r="D47" s="8"/>
       <c r="E47" s="8"/>
       <c r="Q47" s="8"/>
@@ -3672,10 +3688,10 @@
       <c r="T47" s="8"/>
     </row>
     <row r="48" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B48" s="16" t="s">
+      <c r="B48" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="C48" s="16"/>
+      <c r="C48" s="37"/>
       <c r="D48" s="9"/>
       <c r="E48" s="9"/>
       <c r="Q48" s="9"/>
@@ -3684,76 +3700,76 @@
       <c r="T48" s="9"/>
     </row>
     <row r="49" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B49" s="16" t="s">
+      <c r="B49" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="C49" s="16"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="15"/>
-      <c r="Q49" s="15"/>
-      <c r="R49" s="15"/>
-      <c r="S49" s="15"/>
-      <c r="T49" s="15"/>
+      <c r="C49" s="37"/>
+      <c r="D49" s="53"/>
+      <c r="E49" s="53"/>
+      <c r="Q49" s="53"/>
+      <c r="R49" s="53"/>
+      <c r="S49" s="53"/>
+      <c r="T49" s="53"/>
     </row>
     <row r="50" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
-      <c r="D50" s="15"/>
-      <c r="E50" s="15"/>
-      <c r="Q50" s="15"/>
-      <c r="R50" s="15"/>
-      <c r="S50" s="15"/>
-      <c r="T50" s="15"/>
+      <c r="D50" s="53"/>
+      <c r="E50" s="53"/>
+      <c r="Q50" s="53"/>
+      <c r="R50" s="53"/>
+      <c r="S50" s="53"/>
+      <c r="T50" s="53"/>
     </row>
     <row r="51" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B51" s="10"/>
       <c r="C51" s="10"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="15"/>
-      <c r="Q51" s="15"/>
-      <c r="R51" s="15"/>
-      <c r="S51" s="15"/>
-      <c r="T51" s="15"/>
+      <c r="D51" s="53"/>
+      <c r="E51" s="53"/>
+      <c r="Q51" s="53"/>
+      <c r="R51" s="53"/>
+      <c r="S51" s="53"/>
+      <c r="T51" s="53"/>
     </row>
     <row r="52" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B52" s="15"/>
-      <c r="C52" s="15"/>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15"/>
+      <c r="B52" s="53"/>
+      <c r="C52" s="53"/>
+      <c r="D52" s="53"/>
+      <c r="E52" s="53"/>
       <c r="Q52" s="10"/>
       <c r="R52" s="10"/>
-      <c r="S52" s="15"/>
-      <c r="T52" s="15"/>
+      <c r="S52" s="53"/>
+      <c r="T52" s="53"/>
     </row>
     <row r="53" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B53" s="15"/>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="15"/>
+      <c r="B53" s="53"/>
+      <c r="C53" s="53"/>
+      <c r="D53" s="53"/>
+      <c r="E53" s="53"/>
     </row>
     <row r="54" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B54" s="15"/>
-      <c r="C54" s="15"/>
-      <c r="D54" s="15"/>
-      <c r="E54" s="15"/>
+      <c r="B54" s="53"/>
+      <c r="C54" s="53"/>
+      <c r="D54" s="53"/>
+      <c r="E54" s="53"/>
     </row>
     <row r="55" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B55" s="15"/>
-      <c r="C55" s="15"/>
-      <c r="D55" s="15"/>
-      <c r="E55" s="15"/>
+      <c r="B55" s="53"/>
+      <c r="C55" s="53"/>
+      <c r="D55" s="53"/>
+      <c r="E55" s="53"/>
     </row>
     <row r="56" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B56" s="15"/>
-      <c r="C56" s="15"/>
-      <c r="D56" s="15"/>
-      <c r="E56" s="15"/>
+      <c r="B56" s="53"/>
+      <c r="C56" s="53"/>
+      <c r="D56" s="53"/>
+      <c r="E56" s="53"/>
     </row>
     <row r="57" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B57" s="15"/>
-      <c r="C57" s="15"/>
-      <c r="D57" s="15"/>
-      <c r="E57" s="15"/>
+      <c r="B57" s="53"/>
+      <c r="C57" s="53"/>
+      <c r="D57" s="53"/>
+      <c r="E57" s="53"/>
     </row>
     <row r="58" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B58" s="9"/>
@@ -3762,22 +3778,22 @@
       <c r="E58" s="9"/>
     </row>
     <row r="59" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B59" s="15"/>
-      <c r="C59" s="15"/>
-      <c r="D59" s="15"/>
-      <c r="E59" s="15"/>
+      <c r="B59" s="53"/>
+      <c r="C59" s="53"/>
+      <c r="D59" s="53"/>
+      <c r="E59" s="53"/>
     </row>
     <row r="60" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B60" s="15"/>
-      <c r="C60" s="15"/>
-      <c r="D60" s="15"/>
-      <c r="E60" s="15"/>
+      <c r="B60" s="53"/>
+      <c r="C60" s="53"/>
+      <c r="D60" s="53"/>
+      <c r="E60" s="53"/>
     </row>
     <row r="61" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B61" s="10"/>
       <c r="C61" s="10"/>
-      <c r="D61" s="15"/>
-      <c r="E61" s="15"/>
+      <c r="D61" s="53"/>
+      <c r="E61" s="53"/>
     </row>
     <row r="62" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B62" s="10"/>
@@ -3792,30 +3808,313 @@
       <c r="E63" s="9"/>
     </row>
     <row r="154" spans="8:11" x14ac:dyDescent="0.3">
-      <c r="H154" s="34"/>
-      <c r="I154" s="34"/>
-      <c r="J154" s="34"/>
-      <c r="K154" s="34"/>
+      <c r="H154" s="52"/>
+      <c r="I154" s="52"/>
+      <c r="J154" s="52"/>
+      <c r="K154" s="52"/>
     </row>
     <row r="191" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J191" s="34"/>
-      <c r="K191" s="34"/>
+      <c r="J191" s="52"/>
+      <c r="K191" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="333">
-    <mergeCell ref="AE4:AF4"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AG4:AH4"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AJ4:AK4"/>
-    <mergeCell ref="AJ5:AK5"/>
-    <mergeCell ref="AJ6:AK6"/>
-    <mergeCell ref="AJ7:AK7"/>
-    <mergeCell ref="AL4:AM4"/>
-    <mergeCell ref="AL5:AM5"/>
-    <mergeCell ref="AL6:AM6"/>
-    <mergeCell ref="AL7:AM7"/>
-    <mergeCell ref="AG6:AH6"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="E38:F41"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="S49:T49"/>
+    <mergeCell ref="S50:T50"/>
+    <mergeCell ref="S51:T51"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="T28:U28"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="AA4:AB4"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AA6:AB6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="O4:R4"/>
+    <mergeCell ref="O5:R5"/>
+    <mergeCell ref="O6:R6"/>
+    <mergeCell ref="O7:R7"/>
+    <mergeCell ref="O8:R8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="AA7:AB7"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="Q16:R16"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="V18:W18"/>
+    <mergeCell ref="V19:W19"/>
+    <mergeCell ref="V20:W20"/>
+    <mergeCell ref="V21:W21"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="V14:W14"/>
+    <mergeCell ref="V15:W15"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="V13:W13"/>
+    <mergeCell ref="V16:W16"/>
+    <mergeCell ref="V17:W17"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="AK20:AL20"/>
+    <mergeCell ref="AF17:AG17"/>
+    <mergeCell ref="AF18:AG18"/>
+    <mergeCell ref="AF20:AG20"/>
+    <mergeCell ref="AF21:AG21"/>
+    <mergeCell ref="AF22:AG22"/>
+    <mergeCell ref="O13:P24"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="AD13:AE23"/>
+    <mergeCell ref="AF23:AG23"/>
+    <mergeCell ref="AA20:AB20"/>
+    <mergeCell ref="AA21:AB21"/>
+    <mergeCell ref="AA22:AB22"/>
+    <mergeCell ref="AF13:AG13"/>
+    <mergeCell ref="AF14:AG14"/>
+    <mergeCell ref="AF15:AG15"/>
+    <mergeCell ref="AF16:AG16"/>
+    <mergeCell ref="AA13:AB13"/>
+    <mergeCell ref="AA14:AB14"/>
+    <mergeCell ref="AA15:AB15"/>
+    <mergeCell ref="AA16:AB16"/>
+    <mergeCell ref="AA17:AB17"/>
+    <mergeCell ref="AA18:AB18"/>
+    <mergeCell ref="AA19:AB19"/>
+    <mergeCell ref="AA30:AB30"/>
+    <mergeCell ref="AA31:AB31"/>
+    <mergeCell ref="AA32:AB32"/>
+    <mergeCell ref="AA33:AB33"/>
+    <mergeCell ref="AA34:AB34"/>
+    <mergeCell ref="Q31:R31"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="T29:U33"/>
+    <mergeCell ref="V29:W29"/>
+    <mergeCell ref="V32:W32"/>
+    <mergeCell ref="V33:W33"/>
+    <mergeCell ref="V31:W31"/>
+    <mergeCell ref="V30:W30"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="H154:I154"/>
+    <mergeCell ref="T35:U35"/>
+    <mergeCell ref="V35:W35"/>
+    <mergeCell ref="T36:U36"/>
+    <mergeCell ref="V36:W36"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="L35:M35"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="J29:K35"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="Q49:R49"/>
+    <mergeCell ref="Q50:R50"/>
+    <mergeCell ref="Q51:R51"/>
+    <mergeCell ref="AA39:AB39"/>
+    <mergeCell ref="AA40:AB40"/>
+    <mergeCell ref="AA41:AB41"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="Y28:Z28"/>
+    <mergeCell ref="AA28:AB28"/>
+    <mergeCell ref="AA29:AB29"/>
+    <mergeCell ref="Q35:R35"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="Q37:R37"/>
+    <mergeCell ref="L38:M38"/>
+    <mergeCell ref="L39:M39"/>
+    <mergeCell ref="L40:M40"/>
+    <mergeCell ref="L41:M41"/>
+    <mergeCell ref="J38:K41"/>
+    <mergeCell ref="V28:W28"/>
+    <mergeCell ref="V25:W25"/>
+    <mergeCell ref="V22:W22"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="V24:W24"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="AI29:AJ36"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="O29:P37"/>
+    <mergeCell ref="AP13:AQ13"/>
+    <mergeCell ref="AP14:AQ14"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="L37:M37"/>
+    <mergeCell ref="AK31:AL31"/>
+    <mergeCell ref="AK32:AL32"/>
+    <mergeCell ref="AK34:AL34"/>
+    <mergeCell ref="AK33:AL33"/>
+    <mergeCell ref="AK35:AL35"/>
+    <mergeCell ref="AF19:AG19"/>
+    <mergeCell ref="AK16:AL16"/>
+    <mergeCell ref="AD28:AE28"/>
+    <mergeCell ref="AF31:AG31"/>
+    <mergeCell ref="AF30:AG30"/>
+    <mergeCell ref="AF32:AG32"/>
+    <mergeCell ref="AF33:AG33"/>
+    <mergeCell ref="AF34:AG34"/>
+    <mergeCell ref="AF35:AG35"/>
+    <mergeCell ref="AK29:AL29"/>
+    <mergeCell ref="AK30:AL30"/>
+    <mergeCell ref="J191:K191"/>
+    <mergeCell ref="AP29:AQ29"/>
+    <mergeCell ref="AP30:AQ30"/>
+    <mergeCell ref="AP31:AQ31"/>
+    <mergeCell ref="AP32:AQ32"/>
+    <mergeCell ref="AN29:AO32"/>
+    <mergeCell ref="AP33:AQ33"/>
+    <mergeCell ref="AP34:AQ34"/>
+    <mergeCell ref="AP35:AQ35"/>
+    <mergeCell ref="AP38:AQ38"/>
+    <mergeCell ref="AN33:AO38"/>
+    <mergeCell ref="AF36:AG36"/>
+    <mergeCell ref="AD29:AE36"/>
+    <mergeCell ref="AK36:AL36"/>
+    <mergeCell ref="AA42:AB42"/>
+    <mergeCell ref="J154:K154"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="S52:T52"/>
+    <mergeCell ref="Y29:Z42"/>
+    <mergeCell ref="AF29:AG29"/>
+    <mergeCell ref="AA35:AB35"/>
+    <mergeCell ref="AA36:AB36"/>
+    <mergeCell ref="AA37:AB37"/>
+    <mergeCell ref="AA38:AB38"/>
+    <mergeCell ref="AN12:AO12"/>
+    <mergeCell ref="AP12:AQ12"/>
+    <mergeCell ref="AP36:AQ36"/>
+    <mergeCell ref="AP37:AQ37"/>
+    <mergeCell ref="AP18:AQ18"/>
+    <mergeCell ref="AP15:AQ15"/>
+    <mergeCell ref="AP20:AQ20"/>
+    <mergeCell ref="AN13:AO20"/>
+    <mergeCell ref="AP17:AQ17"/>
+    <mergeCell ref="AP16:AQ16"/>
+    <mergeCell ref="AP19:AQ19"/>
+    <mergeCell ref="AN28:AO28"/>
+    <mergeCell ref="AP28:AQ28"/>
+    <mergeCell ref="AF28:AG28"/>
+    <mergeCell ref="AI28:AJ28"/>
+    <mergeCell ref="AK28:AL28"/>
+    <mergeCell ref="AK13:AL13"/>
+    <mergeCell ref="AK15:AL15"/>
+    <mergeCell ref="AK17:AL17"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="T12:U12"/>
+    <mergeCell ref="V12:W12"/>
+    <mergeCell ref="Y12:Z12"/>
+    <mergeCell ref="AA12:AB12"/>
+    <mergeCell ref="AD12:AE12"/>
+    <mergeCell ref="AF12:AG12"/>
+    <mergeCell ref="AI12:AJ12"/>
+    <mergeCell ref="AK12:AL12"/>
+    <mergeCell ref="T13:U25"/>
+    <mergeCell ref="AA23:AB23"/>
+    <mergeCell ref="Y13:Z23"/>
+    <mergeCell ref="AK21:AL21"/>
+    <mergeCell ref="AI13:AJ21"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="AK18:AL18"/>
+    <mergeCell ref="AK14:AL14"/>
+    <mergeCell ref="AK19:AL19"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
@@ -3840,302 +4139,19 @@
     <mergeCell ref="G29:H29"/>
     <mergeCell ref="G23:H23"/>
     <mergeCell ref="G17:H17"/>
-    <mergeCell ref="AF28:AG28"/>
-    <mergeCell ref="AI28:AJ28"/>
-    <mergeCell ref="AK28:AL28"/>
-    <mergeCell ref="AK13:AL13"/>
-    <mergeCell ref="AK15:AL15"/>
-    <mergeCell ref="AK17:AL17"/>
-    <mergeCell ref="Q12:R12"/>
-    <mergeCell ref="T12:U12"/>
-    <mergeCell ref="V12:W12"/>
-    <mergeCell ref="Y12:Z12"/>
-    <mergeCell ref="AA12:AB12"/>
-    <mergeCell ref="AD12:AE12"/>
-    <mergeCell ref="AF12:AG12"/>
-    <mergeCell ref="AI12:AJ12"/>
-    <mergeCell ref="AK12:AL12"/>
-    <mergeCell ref="AN12:AO12"/>
-    <mergeCell ref="AP12:AQ12"/>
-    <mergeCell ref="AP36:AQ36"/>
-    <mergeCell ref="AP37:AQ37"/>
-    <mergeCell ref="AP18:AQ18"/>
-    <mergeCell ref="AP15:AQ15"/>
-    <mergeCell ref="AP20:AQ20"/>
-    <mergeCell ref="AN13:AO20"/>
-    <mergeCell ref="AP17:AQ17"/>
-    <mergeCell ref="AP16:AQ16"/>
-    <mergeCell ref="J191:K191"/>
-    <mergeCell ref="AP29:AQ29"/>
-    <mergeCell ref="AP30:AQ30"/>
-    <mergeCell ref="AP31:AQ31"/>
-    <mergeCell ref="AP32:AQ32"/>
-    <mergeCell ref="AN29:AO32"/>
-    <mergeCell ref="AP33:AQ33"/>
-    <mergeCell ref="AP34:AQ34"/>
-    <mergeCell ref="AP35:AQ35"/>
-    <mergeCell ref="AP38:AQ38"/>
-    <mergeCell ref="AN33:AO38"/>
-    <mergeCell ref="AF36:AG36"/>
-    <mergeCell ref="AD29:AE36"/>
-    <mergeCell ref="AK36:AL36"/>
-    <mergeCell ref="AA42:AB42"/>
-    <mergeCell ref="J154:K154"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="S52:T52"/>
-    <mergeCell ref="AP19:AQ19"/>
-    <mergeCell ref="AN28:AO28"/>
-    <mergeCell ref="AP28:AQ28"/>
-    <mergeCell ref="T13:U25"/>
-    <mergeCell ref="AA23:AB23"/>
-    <mergeCell ref="Y13:Z23"/>
-    <mergeCell ref="AK21:AL21"/>
-    <mergeCell ref="AI13:AJ21"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="AI29:AJ36"/>
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="O29:P37"/>
-    <mergeCell ref="AP13:AQ13"/>
-    <mergeCell ref="AP14:AQ14"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="L37:M37"/>
-    <mergeCell ref="AK31:AL31"/>
-    <mergeCell ref="AK32:AL32"/>
-    <mergeCell ref="AK34:AL34"/>
-    <mergeCell ref="AK33:AL33"/>
-    <mergeCell ref="AK35:AL35"/>
-    <mergeCell ref="AF19:AG19"/>
-    <mergeCell ref="AK16:AL16"/>
-    <mergeCell ref="AD28:AE28"/>
-    <mergeCell ref="AF31:AG31"/>
-    <mergeCell ref="AF30:AG30"/>
-    <mergeCell ref="AF32:AG32"/>
-    <mergeCell ref="AF33:AG33"/>
-    <mergeCell ref="AF34:AG34"/>
-    <mergeCell ref="AF35:AG35"/>
-    <mergeCell ref="AK29:AL29"/>
-    <mergeCell ref="AK30:AL30"/>
-    <mergeCell ref="Y29:Z42"/>
-    <mergeCell ref="AF29:AG29"/>
-    <mergeCell ref="AA35:AB35"/>
-    <mergeCell ref="AA36:AB36"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="AA37:AB37"/>
-    <mergeCell ref="AA38:AB38"/>
-    <mergeCell ref="AA39:AB39"/>
-    <mergeCell ref="AA40:AB40"/>
-    <mergeCell ref="AA41:AB41"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="Y28:Z28"/>
-    <mergeCell ref="AA28:AB28"/>
-    <mergeCell ref="AA29:AB29"/>
-    <mergeCell ref="Q35:R35"/>
-    <mergeCell ref="Q36:R36"/>
-    <mergeCell ref="Q37:R37"/>
-    <mergeCell ref="L38:M38"/>
-    <mergeCell ref="L39:M39"/>
-    <mergeCell ref="L40:M40"/>
-    <mergeCell ref="L41:M41"/>
-    <mergeCell ref="J38:K41"/>
-    <mergeCell ref="V28:W28"/>
-    <mergeCell ref="V25:W25"/>
-    <mergeCell ref="V22:W22"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="V24:W24"/>
-    <mergeCell ref="H154:I154"/>
-    <mergeCell ref="T35:U35"/>
-    <mergeCell ref="V35:W35"/>
-    <mergeCell ref="T36:U36"/>
-    <mergeCell ref="V36:W36"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="L34:M34"/>
-    <mergeCell ref="L35:M35"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="J29:K35"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="AA30:AB30"/>
-    <mergeCell ref="AA31:AB31"/>
-    <mergeCell ref="AA32:AB32"/>
-    <mergeCell ref="AA33:AB33"/>
-    <mergeCell ref="AA34:AB34"/>
-    <mergeCell ref="Q31:R31"/>
-    <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="Q33:R33"/>
-    <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="T29:U33"/>
-    <mergeCell ref="V29:W29"/>
-    <mergeCell ref="V32:W32"/>
-    <mergeCell ref="V33:W33"/>
-    <mergeCell ref="V31:W31"/>
-    <mergeCell ref="V30:W30"/>
-    <mergeCell ref="Q30:R30"/>
-    <mergeCell ref="AK18:AL18"/>
-    <mergeCell ref="AK14:AL14"/>
-    <mergeCell ref="AK19:AL19"/>
-    <mergeCell ref="AK20:AL20"/>
-    <mergeCell ref="AF17:AG17"/>
-    <mergeCell ref="AF18:AG18"/>
-    <mergeCell ref="AF20:AG20"/>
-    <mergeCell ref="AF21:AG21"/>
-    <mergeCell ref="AF22:AG22"/>
-    <mergeCell ref="O13:P24"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="AD13:AE23"/>
-    <mergeCell ref="AF23:AG23"/>
-    <mergeCell ref="AA20:AB20"/>
-    <mergeCell ref="AA21:AB21"/>
-    <mergeCell ref="AA22:AB22"/>
-    <mergeCell ref="AF13:AG13"/>
-    <mergeCell ref="AF14:AG14"/>
-    <mergeCell ref="AF15:AG15"/>
-    <mergeCell ref="AF16:AG16"/>
-    <mergeCell ref="AA13:AB13"/>
-    <mergeCell ref="AA14:AB14"/>
-    <mergeCell ref="AA15:AB15"/>
-    <mergeCell ref="AA16:AB16"/>
-    <mergeCell ref="AA17:AB17"/>
-    <mergeCell ref="AA18:AB18"/>
-    <mergeCell ref="AA19:AB19"/>
-    <mergeCell ref="V18:W18"/>
-    <mergeCell ref="V19:W19"/>
-    <mergeCell ref="V20:W20"/>
-    <mergeCell ref="V21:W21"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="V14:W14"/>
-    <mergeCell ref="V15:W15"/>
-    <mergeCell ref="Q20:R20"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="V13:W13"/>
-    <mergeCell ref="V16:W16"/>
-    <mergeCell ref="V17:W17"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="Q16:R16"/>
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="AA4:AB4"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AA6:AB6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="O4:R4"/>
-    <mergeCell ref="O5:R5"/>
-    <mergeCell ref="O6:R6"/>
-    <mergeCell ref="O7:R7"/>
-    <mergeCell ref="O8:R8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="Q49:R49"/>
-    <mergeCell ref="Q50:R50"/>
-    <mergeCell ref="Q51:R51"/>
-    <mergeCell ref="S9:T9"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="S49:T49"/>
-    <mergeCell ref="S50:T50"/>
-    <mergeCell ref="S51:T51"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="T28:U28"/>
-    <mergeCell ref="AA7:AB7"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="E38:F41"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AJ4:AK4"/>
+    <mergeCell ref="AJ5:AK5"/>
+    <mergeCell ref="AJ6:AK6"/>
+    <mergeCell ref="AJ7:AK7"/>
+    <mergeCell ref="AL4:AM4"/>
+    <mergeCell ref="AL5:AM5"/>
+    <mergeCell ref="AL6:AM6"/>
+    <mergeCell ref="AL7:AM7"/>
+    <mergeCell ref="AG6:AH6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4146,8 +4162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
@@ -4156,245 +4172,245 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
       <c r="K1" s="10"/>
     </row>
     <row r="2" spans="1:31" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="65"/>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="69" t="s">
+      <c r="A2" s="16"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="85" t="s">
         <v>208</v>
       </c>
-      <c r="M2" s="70"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71"/>
-      <c r="Q2" s="71"/>
-      <c r="R2" s="71"/>
-      <c r="S2" s="71"/>
-      <c r="T2" s="71"/>
-      <c r="U2" s="71"/>
-      <c r="V2" s="71"/>
-      <c r="W2" s="72"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="21"/>
     </row>
     <row r="3" spans="1:31" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="65"/>
-      <c r="B3" s="66"/>
-      <c r="C3" s="48" t="s">
+      <c r="A3" s="16"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="76" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
       <c r="F3" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="68"/>
-      <c r="L3" s="74"/>
-      <c r="M3" s="75"/>
-      <c r="N3" s="75"/>
-      <c r="O3" s="75"/>
-      <c r="P3" s="75"/>
-      <c r="Q3" s="75"/>
-      <c r="R3" s="75"/>
-      <c r="S3" s="76"/>
-      <c r="T3" s="77"/>
-      <c r="U3" s="77"/>
-      <c r="V3" s="77"/>
-      <c r="W3" s="78"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
+      <c r="Q3" s="24"/>
+      <c r="R3" s="24"/>
+      <c r="S3" s="25"/>
+      <c r="T3" s="26"/>
+      <c r="U3" s="26"/>
+      <c r="V3" s="26"/>
+      <c r="W3" s="27"/>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A4" s="65"/>
-      <c r="B4" s="66"/>
-      <c r="C4" s="50" t="s">
+      <c r="A4" s="16"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
       <c r="F4" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="73"/>
-      <c r="K4" s="68"/>
-      <c r="L4" s="79"/>
-      <c r="M4" s="62" t="s">
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="88" t="s">
         <v>209</v>
       </c>
-      <c r="N4" s="63"/>
+      <c r="N4" s="89"/>
       <c r="O4" s="80" t="s">
         <v>50</v>
       </c>
       <c r="P4" s="80"/>
       <c r="Q4" s="80"/>
       <c r="R4" s="81"/>
-      <c r="S4" s="76"/>
-      <c r="T4" s="23" t="s">
+      <c r="S4" s="25"/>
+      <c r="T4" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="U4" s="23"/>
+      <c r="U4" s="60"/>
       <c r="V4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="W4" s="78"/>
-      <c r="Y4" s="17" t="s">
+      <c r="W4" s="27"/>
+      <c r="Y4" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="Z4" s="17"/>
+      <c r="Z4" s="43"/>
       <c r="AA4" s="3" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A5" s="65"/>
-      <c r="B5" s="66"/>
-      <c r="C5" s="51" t="s">
+      <c r="A5" s="16"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="79" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
       <c r="F5" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="73"/>
-      <c r="K5" s="68"/>
-      <c r="L5" s="79"/>
-      <c r="M5" s="56" t="s">
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="73" t="s">
         <v>47</v>
       </c>
-      <c r="N5" s="57"/>
-      <c r="O5" s="57" t="s">
+      <c r="N5" s="74"/>
+      <c r="O5" s="74" t="s">
         <v>49</v>
       </c>
-      <c r="P5" s="57"/>
-      <c r="Q5" s="57"/>
-      <c r="R5" s="58"/>
-      <c r="S5" s="76"/>
-      <c r="T5" s="16" t="s">
+      <c r="P5" s="74"/>
+      <c r="Q5" s="74"/>
+      <c r="R5" s="75"/>
+      <c r="S5" s="25"/>
+      <c r="T5" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="U5" s="16"/>
+      <c r="U5" s="37"/>
       <c r="V5" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="W5" s="78"/>
-      <c r="Y5" s="88" t="s">
+      <c r="W5" s="27"/>
+      <c r="Y5" s="70" t="s">
         <v>47</v>
       </c>
-      <c r="Z5" s="88"/>
+      <c r="Z5" s="70"/>
       <c r="AA5" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A6" s="65"/>
-      <c r="B6" s="66"/>
-      <c r="C6" s="52" t="s">
+      <c r="A6" s="16"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
       <c r="F6" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="66"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="66"/>
-      <c r="J6" s="73"/>
-      <c r="K6" s="68"/>
-      <c r="L6" s="79"/>
-      <c r="M6" s="20" t="s">
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16" t="s">
+      <c r="N6" s="37"/>
+      <c r="O6" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="47"/>
-      <c r="S6" s="76"/>
-      <c r="T6" s="16" t="s">
+      <c r="P6" s="37"/>
+      <c r="Q6" s="37"/>
+      <c r="R6" s="84"/>
+      <c r="S6" s="25"/>
+      <c r="T6" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="U6" s="16"/>
+      <c r="U6" s="37"/>
       <c r="V6" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="W6" s="78"/>
-      <c r="Y6" s="89" t="s">
+      <c r="W6" s="27"/>
+      <c r="Y6" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="Z6" s="89"/>
+      <c r="Z6" s="71"/>
       <c r="AA6" s="3" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A7" s="65"/>
-      <c r="B7" s="66"/>
-      <c r="C7" s="53" t="s">
+      <c r="A7" s="16"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="67" t="s">
         <v>71</v>
       </c>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
       <c r="F7" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="66"/>
-      <c r="H7" s="66"/>
-      <c r="I7" s="66"/>
-      <c r="J7" s="73"/>
-      <c r="K7" s="68"/>
-      <c r="L7" s="79"/>
-      <c r="M7" s="56" t="s">
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="73" t="s">
         <v>206</v>
       </c>
-      <c r="N7" s="57"/>
-      <c r="O7" s="57" t="s">
+      <c r="N7" s="74"/>
+      <c r="O7" s="74" t="s">
         <v>202</v>
       </c>
-      <c r="P7" s="57"/>
-      <c r="Q7" s="57"/>
-      <c r="R7" s="58"/>
-      <c r="S7" s="76"/>
-      <c r="T7" s="16" t="s">
+      <c r="P7" s="74"/>
+      <c r="Q7" s="74"/>
+      <c r="R7" s="75"/>
+      <c r="S7" s="25"/>
+      <c r="T7" s="37" t="s">
         <v>210</v>
       </c>
-      <c r="U7" s="16"/>
+      <c r="U7" s="37"/>
       <c r="V7" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="W7" s="78"/>
-      <c r="Y7" s="45" t="s">
+      <c r="W7" s="27"/>
+      <c r="Y7" s="72" t="s">
         <v>50</v>
       </c>
-      <c r="Z7" s="45"/>
+      <c r="Z7" s="72"/>
       <c r="AA7" s="3" t="s">
         <v>60</v>
       </c>
@@ -4403,62 +4419,62 @@
       </c>
     </row>
     <row r="8" spans="1:31" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="65"/>
-      <c r="B8" s="66"/>
-      <c r="C8" s="54" t="s">
+      <c r="A8" s="16"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="68" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
       <c r="F8" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="G8" s="66"/>
-      <c r="H8" s="66"/>
-      <c r="I8" s="66"/>
-      <c r="J8" s="73"/>
-      <c r="K8" s="68"/>
-      <c r="L8" s="79"/>
-      <c r="M8" s="59" t="s">
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="87" t="s">
         <v>207</v>
       </c>
-      <c r="N8" s="60"/>
-      <c r="O8" s="60" t="s">
+      <c r="N8" s="82"/>
+      <c r="O8" s="82" t="s">
         <v>202</v>
       </c>
-      <c r="P8" s="60"/>
-      <c r="Q8" s="60"/>
-      <c r="R8" s="61"/>
-      <c r="S8" s="76"/>
-      <c r="T8" s="76"/>
-      <c r="U8" s="76"/>
-      <c r="V8" s="76"/>
-      <c r="W8" s="78"/>
+      <c r="P8" s="82"/>
+      <c r="Q8" s="82"/>
+      <c r="R8" s="83"/>
+      <c r="S8" s="25"/>
+      <c r="T8" s="25"/>
+      <c r="U8" s="25"/>
+      <c r="V8" s="25"/>
+      <c r="W8" s="27"/>
     </row>
     <row r="9" spans="1:31" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="65"/>
-      <c r="B9" s="82"/>
-      <c r="C9" s="83"/>
-      <c r="D9" s="83"/>
-      <c r="E9" s="83"/>
-      <c r="F9" s="83"/>
-      <c r="G9" s="83"/>
-      <c r="H9" s="83"/>
-      <c r="I9" s="83"/>
-      <c r="J9" s="84"/>
-      <c r="K9" s="68"/>
-      <c r="L9" s="85"/>
-      <c r="M9" s="86"/>
-      <c r="N9" s="86"/>
-      <c r="O9" s="86"/>
-      <c r="P9" s="86"/>
-      <c r="Q9" s="86"/>
-      <c r="R9" s="86"/>
-      <c r="S9" s="86"/>
-      <c r="T9" s="86"/>
-      <c r="U9" s="86"/>
-      <c r="V9" s="86"/>
-      <c r="W9" s="87"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="33"/>
+      <c r="O9" s="33"/>
+      <c r="P9" s="33"/>
+      <c r="Q9" s="33"/>
+      <c r="R9" s="33"/>
+      <c r="S9" s="33"/>
+      <c r="T9" s="33"/>
+      <c r="U9" s="33"/>
+      <c r="V9" s="33"/>
+      <c r="W9" s="34"/>
     </row>
     <row r="10" spans="1:31" ht="17.399999999999999" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B10" s="10"/>
@@ -4485,297 +4501,241 @@
       <c r="K11" s="10"/>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="30"/>
-      <c r="E14" s="24" t="s">
+      <c r="D14" s="59"/>
+      <c r="E14" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="I14" s="25" t="s">
+      <c r="F14" s="55"/>
+      <c r="G14" s="55"/>
+      <c r="I14" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="J14" s="25"/>
-      <c r="K14" s="24" t="s">
+      <c r="J14" s="61"/>
+      <c r="K14" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="L14" s="24"/>
-      <c r="M14" s="24"/>
-      <c r="N14" s="24"/>
-      <c r="P14" s="46" t="s">
+      <c r="L14" s="55"/>
+      <c r="M14" s="55"/>
+      <c r="N14" s="55"/>
+      <c r="P14" s="90" t="s">
         <v>63</v>
       </c>
-      <c r="Q14" s="46"/>
-      <c r="R14" s="24" t="s">
+      <c r="Q14" s="90"/>
+      <c r="R14" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="S14" s="24"/>
-      <c r="T14" s="24"/>
-      <c r="U14" s="24"/>
-      <c r="W14" s="31" t="s">
+      <c r="S14" s="55"/>
+      <c r="T14" s="55"/>
+      <c r="U14" s="55"/>
+      <c r="W14" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="X14" s="31"/>
-      <c r="Y14" s="16" t="s">
+      <c r="X14" s="35"/>
+      <c r="Y14" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="Z14" s="16"/>
-      <c r="AB14" s="43" t="s">
+      <c r="Z14" s="37"/>
+      <c r="AB14" s="36" t="s">
         <v>205</v>
       </c>
-      <c r="AC14" s="43"/>
-      <c r="AD14" s="16" t="s">
+      <c r="AC14" s="36"/>
+      <c r="AD14" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="AE14" s="16"/>
+      <c r="AE14" s="37"/>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16" t="s">
+      <c r="D15" s="37"/>
+      <c r="E15" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="I15" s="26" t="s">
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="I15" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="J15" s="26"/>
-      <c r="K15" s="16" t="s">
+      <c r="J15" s="62"/>
+      <c r="K15" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
-      <c r="N15" s="16"/>
-      <c r="P15" s="26" t="s">
+      <c r="L15" s="37"/>
+      <c r="M15" s="37"/>
+      <c r="N15" s="37"/>
+      <c r="P15" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="Q15" s="26"/>
-      <c r="R15" s="16" t="s">
+      <c r="Q15" s="62"/>
+      <c r="R15" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="S15" s="16"/>
-      <c r="T15" s="16"/>
-      <c r="U15" s="16"/>
-      <c r="W15" s="43" t="s">
+      <c r="S15" s="37"/>
+      <c r="T15" s="37"/>
+      <c r="U15" s="37"/>
+      <c r="W15" s="36" t="s">
         <v>205</v>
       </c>
-      <c r="X15" s="43"/>
-      <c r="Y15" s="16" t="s">
+      <c r="X15" s="36"/>
+      <c r="Y15" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="Z15" s="16"/>
-      <c r="AB15" s="16" t="s">
+      <c r="Z15" s="37"/>
+      <c r="AB15" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="AC15" s="16"/>
-      <c r="AD15" s="16" t="s">
+      <c r="AC15" s="37"/>
+      <c r="AD15" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="AE15" s="16"/>
+      <c r="AE15" s="37"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16" t="s">
+      <c r="D16" s="37"/>
+      <c r="E16" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="I16" s="16" t="s">
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="I16" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16" t="s">
+      <c r="J16" s="37"/>
+      <c r="K16" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
-      <c r="N16" s="16"/>
-      <c r="P16" s="45" t="s">
+      <c r="L16" s="37"/>
+      <c r="M16" s="37"/>
+      <c r="N16" s="37"/>
+      <c r="P16" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="Q16" s="45"/>
-      <c r="R16" s="16" t="s">
+      <c r="Q16" s="72"/>
+      <c r="R16" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="S16" s="16"/>
-      <c r="T16" s="16"/>
-      <c r="U16" s="16"/>
-      <c r="AB16" s="16" t="s">
+      <c r="S16" s="37"/>
+      <c r="T16" s="37"/>
+      <c r="U16" s="37"/>
+      <c r="AB16" s="37" t="s">
         <v>200</v>
       </c>
-      <c r="AC16" s="16"/>
-      <c r="AD16" s="16" t="s">
+      <c r="AC16" s="37"/>
+      <c r="AD16" s="37" t="s">
         <v>203</v>
       </c>
-      <c r="AE16" s="16"/>
+      <c r="AE16" s="37"/>
     </row>
     <row r="17" spans="3:31" x14ac:dyDescent="0.3">
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17" t="s">
+      <c r="D17" s="43"/>
+      <c r="E17" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="I17" s="16" t="s">
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="I17" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16" t="s">
+      <c r="J17" s="37"/>
+      <c r="K17" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="L17" s="16"/>
-      <c r="M17" s="16"/>
-      <c r="N17" s="16"/>
-      <c r="P17" s="22" t="s">
+      <c r="L17" s="37"/>
+      <c r="M17" s="37"/>
+      <c r="N17" s="37"/>
+      <c r="P17" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="Q17" s="22"/>
-      <c r="R17" s="16" t="s">
+      <c r="Q17" s="44"/>
+      <c r="R17" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="S17" s="16"/>
-      <c r="T17" s="16"/>
-      <c r="U17" s="16"/>
-      <c r="AB17" s="16" t="s">
+      <c r="S17" s="37"/>
+      <c r="T17" s="37"/>
+      <c r="U17" s="37"/>
+      <c r="AB17" s="37" t="s">
         <v>201</v>
       </c>
-      <c r="AC17" s="16"/>
-      <c r="AD17" s="16" t="s">
+      <c r="AC17" s="37"/>
+      <c r="AD17" s="37" t="s">
         <v>202</v>
       </c>
-      <c r="AE17" s="16"/>
+      <c r="AE17" s="37"/>
     </row>
     <row r="18" spans="3:31" x14ac:dyDescent="0.3">
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17" t="s">
+      <c r="D18" s="43"/>
+      <c r="E18" s="91" t="s">
         <v>65</v>
       </c>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="I18" s="16" t="s">
+      <c r="F18" s="91"/>
+      <c r="G18" s="91"/>
+      <c r="I18" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16" t="s">
+      <c r="J18" s="37"/>
+      <c r="K18" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="L18" s="16"/>
-      <c r="M18" s="16"/>
-      <c r="N18" s="16"/>
-      <c r="P18" s="16" t="s">
+      <c r="L18" s="37"/>
+      <c r="M18" s="37"/>
+      <c r="N18" s="37"/>
+      <c r="P18" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="Q18" s="16"/>
-      <c r="R18" s="16" t="s">
+      <c r="Q18" s="37"/>
+      <c r="R18" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="S18" s="16"/>
-      <c r="T18" s="16"/>
-      <c r="U18" s="16"/>
+      <c r="S18" s="37"/>
+      <c r="T18" s="37"/>
+      <c r="U18" s="37"/>
     </row>
     <row r="19" spans="3:31" x14ac:dyDescent="0.3">
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16" t="s">
+      <c r="D19" s="37"/>
+      <c r="E19" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
     </row>
     <row r="20" spans="3:31" x14ac:dyDescent="0.3">
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16" t="s">
+      <c r="D20" s="37"/>
+      <c r="E20" s="37" t="s">
+        <v>213</v>
+      </c>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+      <c r="N20" s="65" t="s">
         <v>212</v>
       </c>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="N20" s="90" t="s">
-        <v>213</v>
-      </c>
-      <c r="O20" s="90"/>
-      <c r="P20" s="90"/>
+      <c r="O20" s="65"/>
+      <c r="P20" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="72">
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="N20:P20"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="Y4:Z4"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="Y6:Z6"/>
-    <mergeCell ref="Y7:Z7"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="O5:R5"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="O4:R4"/>
-    <mergeCell ref="O7:R7"/>
-    <mergeCell ref="O8:R8"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="T7:U7"/>
-    <mergeCell ref="O6:R6"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="K14:N14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="K18:N18"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="K15:N15"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K16:N16"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="K17:N17"/>
-    <mergeCell ref="R14:U14"/>
-    <mergeCell ref="R15:U15"/>
-    <mergeCell ref="R16:U16"/>
-    <mergeCell ref="R17:U17"/>
-    <mergeCell ref="R18:U18"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="E20:H20"/>
     <mergeCell ref="AB16:AC16"/>
     <mergeCell ref="AD16:AE16"/>
     <mergeCell ref="AB17:AC17"/>
@@ -4788,6 +4748,64 @@
     <mergeCell ref="AD14:AE14"/>
     <mergeCell ref="AB15:AC15"/>
     <mergeCell ref="AD15:AE15"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="R14:U14"/>
+    <mergeCell ref="R15:U15"/>
+    <mergeCell ref="R16:U16"/>
+    <mergeCell ref="R17:U17"/>
+    <mergeCell ref="R18:U18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="K15:N15"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K16:N16"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="K17:N17"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="K14:N14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="O4:R4"/>
+    <mergeCell ref="O7:R7"/>
+    <mergeCell ref="O6:R6"/>
+    <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="Y6:Z6"/>
+    <mergeCell ref="Y7:Z7"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O5:R5"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="T7:U7"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="O8:R8"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="K18:N18"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="C18:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>